<commit_message>
Update backend logic, market data, and stock files
🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/dumps/Stocks/Afcons Infrastructure Ltd.xlsx
+++ b/dumps/Stocks/Afcons Infrastructure Ltd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lenin/Desktop/workspace/pl/dumps/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54496614-E428-944D-9BB3-D003589E5B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2432D2AE-2B10-D940-8A0D-094401A9543E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="19880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="79">
   <si>
     <t>UnRealised</t>
   </si>
@@ -873,13 +873,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AP1001"/>
+  <dimension ref="A1:AP1002"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
-      <pane xSplit="6" ySplit="4" topLeftCell="G22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="4" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G36" sqref="G36"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1188,7 +1188,7 @@
     </row>
     <row r="6" spans="1:42" ht="15.75" customHeight="1">
       <c r="A6" s="55">
-        <v>46059</v>
+        <v>46062</v>
       </c>
       <c r="B6" t="s">
         <v>26</v>
@@ -1200,10 +1200,10 @@
         <v>10</v>
       </c>
       <c r="E6">
-        <v>333.4</v>
+        <v>338.08</v>
       </c>
       <c r="F6">
-        <v>3350.7</v>
+        <v>3380.8</v>
       </c>
       <c r="G6" t="s">
         <v>29</v>
@@ -1218,7 +1218,7 @@
     </row>
     <row r="7" spans="1:42" ht="15.75" customHeight="1">
       <c r="A7" s="55">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="B7" t="s">
         <v>26</v>
@@ -1230,16 +1230,16 @@
         <v>10</v>
       </c>
       <c r="E7">
-        <v>339.9</v>
+        <v>333.4</v>
       </c>
       <c r="F7">
-        <v>3416</v>
+        <v>3350.7</v>
       </c>
       <c r="G7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I7">
-        <v>17</v>
+        <v>16.7</v>
       </c>
       <c r="J7">
         <f>Index!$C$2</f>
@@ -1248,7 +1248,7 @@
     </row>
     <row r="8" spans="1:42" ht="15.75" customHeight="1">
       <c r="A8" s="55">
-        <v>46050</v>
+        <v>46057</v>
       </c>
       <c r="B8" t="s">
         <v>26</v>
@@ -1260,13 +1260,13 @@
         <v>10</v>
       </c>
       <c r="E8">
-        <v>339.1</v>
+        <v>339.9</v>
       </c>
       <c r="F8">
-        <v>3408</v>
+        <v>3416</v>
       </c>
       <c r="G8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I8">
         <v>17</v>
@@ -1276,9 +1276,9 @@
         <v>338.15</v>
       </c>
     </row>
-    <row r="9" spans="1:42" ht="13" customHeight="1">
+    <row r="9" spans="1:42" ht="15.75" customHeight="1">
       <c r="A9" s="55">
-        <v>46049</v>
+        <v>46050</v>
       </c>
       <c r="B9" t="s">
         <v>26</v>
@@ -1290,16 +1290,16 @@
         <v>10</v>
       </c>
       <c r="E9">
-        <v>337.8</v>
+        <v>339.1</v>
       </c>
       <c r="F9">
-        <v>3394.9</v>
+        <v>3408</v>
       </c>
       <c r="G9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I9">
-        <v>16.899999999999999</v>
+        <v>17</v>
       </c>
       <c r="J9">
         <f>Index!$C$2</f>
@@ -1308,7 +1308,7 @@
     </row>
     <row r="10" spans="1:42" ht="13" customHeight="1">
       <c r="A10" s="55">
-        <v>46034</v>
+        <v>46049</v>
       </c>
       <c r="B10" t="s">
         <v>26</v>
@@ -1317,19 +1317,19 @@
         <v>27</v>
       </c>
       <c r="D10">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E10">
-        <v>356.85</v>
+        <v>337.8</v>
       </c>
       <c r="F10">
-        <v>7172.6</v>
+        <v>3394.9</v>
       </c>
       <c r="G10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I10">
-        <v>35.6</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="J10">
         <f>Index!$C$2</f>
@@ -1338,7 +1338,7 @@
     </row>
     <row r="11" spans="1:42" ht="13" customHeight="1">
       <c r="A11" s="55">
-        <v>46030</v>
+        <v>46034</v>
       </c>
       <c r="B11" t="s">
         <v>26</v>
@@ -1347,19 +1347,19 @@
         <v>27</v>
       </c>
       <c r="D11">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E11">
-        <v>379.65</v>
+        <v>356.85</v>
       </c>
       <c r="F11">
-        <v>3815.5</v>
+        <v>7172.6</v>
       </c>
       <c r="G11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I11">
-        <v>19</v>
+        <v>35.6</v>
       </c>
       <c r="J11">
         <f>Index!$C$2</f>
@@ -1368,7 +1368,7 @@
     </row>
     <row r="12" spans="1:42" ht="13" customHeight="1">
       <c r="A12" s="55">
-        <v>46027</v>
+        <v>46030</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
@@ -1380,16 +1380,16 @@
         <v>10</v>
       </c>
       <c r="E12">
-        <v>388.6</v>
+        <v>379.65</v>
       </c>
       <c r="F12">
-        <v>3905.4</v>
+        <v>3815.5</v>
       </c>
       <c r="G12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I12">
-        <v>19.399999999999999</v>
+        <v>19</v>
       </c>
       <c r="J12">
         <f>Index!$C$2</f>
@@ -1398,7 +1398,7 @@
     </row>
     <row r="13" spans="1:42" ht="13" customHeight="1">
       <c r="A13" s="55">
-        <v>46024</v>
+        <v>46027</v>
       </c>
       <c r="B13" t="s">
         <v>26</v>
@@ -1410,16 +1410,16 @@
         <v>10</v>
       </c>
       <c r="E13">
-        <v>391.25</v>
+        <v>388.6</v>
       </c>
       <c r="F13">
-        <v>3932.1</v>
+        <v>3905.4</v>
       </c>
       <c r="G13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I13">
-        <v>19.600000000000001</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="J13">
         <f>Index!$C$2</f>
@@ -1428,7 +1428,7 @@
     </row>
     <row r="14" spans="1:42" ht="13" customHeight="1">
       <c r="A14" s="55">
-        <v>46022</v>
+        <v>46024</v>
       </c>
       <c r="B14" t="s">
         <v>26</v>
@@ -1440,16 +1440,16 @@
         <v>10</v>
       </c>
       <c r="E14">
-        <v>390</v>
+        <v>391.25</v>
       </c>
       <c r="F14">
-        <v>3919.5</v>
+        <v>3932.1</v>
       </c>
       <c r="G14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I14">
-        <v>19.5</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="J14">
         <f>Index!$C$2</f>
@@ -1458,7 +1458,7 @@
     </row>
     <row r="15" spans="1:42" ht="13" customHeight="1">
       <c r="A15" s="55">
-        <v>46020</v>
+        <v>46022</v>
       </c>
       <c r="B15" t="s">
         <v>26</v>
@@ -1470,16 +1470,16 @@
         <v>10</v>
       </c>
       <c r="E15">
-        <v>385.8</v>
+        <v>390</v>
       </c>
       <c r="F15">
-        <v>3877.3</v>
+        <v>3919.5</v>
       </c>
       <c r="G15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I15">
-        <v>19.3</v>
+        <v>19.5</v>
       </c>
       <c r="J15">
         <f>Index!$C$2</f>
@@ -1488,7 +1488,7 @@
     </row>
     <row r="16" spans="1:42" ht="13" customHeight="1">
       <c r="A16" s="55">
-        <v>46017</v>
+        <v>46020</v>
       </c>
       <c r="B16" t="s">
         <v>26</v>
@@ -1497,19 +1497,19 @@
         <v>27</v>
       </c>
       <c r="D16">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E16">
-        <v>390.7</v>
+        <v>385.8</v>
       </c>
       <c r="F16">
-        <v>7853</v>
+        <v>3877.3</v>
       </c>
       <c r="G16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I16">
-        <v>39</v>
+        <v>19.3</v>
       </c>
       <c r="J16">
         <f>Index!$C$2</f>
@@ -1518,7 +1518,7 @@
     </row>
     <row r="17" spans="1:10" ht="13" customHeight="1">
       <c r="A17" s="55">
-        <v>46015</v>
+        <v>46017</v>
       </c>
       <c r="B17" t="s">
         <v>26</v>
@@ -1527,19 +1527,19 @@
         <v>27</v>
       </c>
       <c r="D17">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E17">
-        <v>386.65</v>
+        <v>390.7</v>
       </c>
       <c r="F17">
-        <v>3885.8</v>
+        <v>7853</v>
       </c>
       <c r="G17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I17">
-        <v>19.3</v>
+        <v>39</v>
       </c>
       <c r="J17">
         <f>Index!$C$2</f>
@@ -1548,7 +1548,7 @@
     </row>
     <row r="18" spans="1:10" ht="13" customHeight="1">
       <c r="A18" s="55">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B18" t="s">
         <v>26</v>
@@ -1560,16 +1560,16 @@
         <v>10</v>
       </c>
       <c r="E18">
-        <v>382</v>
+        <v>386.65</v>
       </c>
       <c r="F18">
-        <v>3839.1</v>
+        <v>3885.8</v>
       </c>
       <c r="G18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I18">
-        <v>19.100000000000001</v>
+        <v>19.3</v>
       </c>
       <c r="J18">
         <f>Index!$C$2</f>
@@ -1578,7 +1578,7 @@
     </row>
     <row r="19" spans="1:10" ht="13" customHeight="1">
       <c r="A19" s="55">
-        <v>46009</v>
+        <v>46014</v>
       </c>
       <c r="B19" t="s">
         <v>26</v>
@@ -1590,16 +1590,16 @@
         <v>10</v>
       </c>
       <c r="E19">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F19">
-        <v>3849.2</v>
+        <v>3839.1</v>
       </c>
       <c r="G19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I19">
-        <v>19.2</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="J19">
         <f>Index!$C$2</f>
@@ -1608,7 +1608,7 @@
     </row>
     <row r="20" spans="1:10" ht="13" customHeight="1">
       <c r="A20" s="55">
-        <v>46007</v>
+        <v>46009</v>
       </c>
       <c r="B20" t="s">
         <v>26</v>
@@ -1620,16 +1620,16 @@
         <v>10</v>
       </c>
       <c r="E20">
-        <v>396.15</v>
+        <v>383</v>
       </c>
       <c r="F20">
-        <v>3981.3</v>
+        <v>3849.2</v>
       </c>
       <c r="G20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I20">
-        <v>19.8</v>
+        <v>19.2</v>
       </c>
       <c r="J20">
         <f>Index!$C$2</f>
@@ -1638,7 +1638,7 @@
     </row>
     <row r="21" spans="1:10" ht="13" customHeight="1">
       <c r="A21" s="55">
-        <v>46002</v>
+        <v>46007</v>
       </c>
       <c r="B21" t="s">
         <v>26</v>
@@ -1647,19 +1647,19 @@
         <v>27</v>
       </c>
       <c r="D21">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E21">
-        <v>396.45</v>
+        <v>396.15</v>
       </c>
       <c r="F21">
-        <v>7968.6</v>
+        <v>3981.3</v>
       </c>
       <c r="G21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I21">
-        <v>39.6</v>
+        <v>19.8</v>
       </c>
       <c r="J21">
         <f>Index!$C$2</f>
@@ -1668,28 +1668,28 @@
     </row>
     <row r="22" spans="1:10" ht="13" customHeight="1">
       <c r="A22" s="55">
-        <v>45996</v>
+        <v>46002</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="C22" t="s">
         <v>27</v>
       </c>
       <c r="D22">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E22">
-        <v>399.05</v>
+        <v>396.45</v>
       </c>
       <c r="F22">
-        <v>4010.5</v>
+        <v>7968.6</v>
       </c>
       <c r="G22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I22">
-        <v>20</v>
+        <v>39.6</v>
       </c>
       <c r="J22">
         <f>Index!$C$2</f>
@@ -1698,7 +1698,7 @@
     </row>
     <row r="23" spans="1:10" ht="13" customHeight="1">
       <c r="A23" s="55">
-        <v>45993</v>
+        <v>45996</v>
       </c>
       <c r="B23" t="s">
         <v>45</v>
@@ -1710,16 +1710,16 @@
         <v>10</v>
       </c>
       <c r="E23">
-        <v>411.5</v>
+        <v>399.05</v>
       </c>
       <c r="F23">
-        <v>4135.6000000000004</v>
+        <v>4010.5</v>
       </c>
       <c r="G23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I23">
-        <v>20.6</v>
+        <v>20</v>
       </c>
       <c r="J23">
         <f>Index!$C$2</f>
@@ -1728,10 +1728,10 @@
     </row>
     <row r="24" spans="1:10" ht="13" customHeight="1">
       <c r="A24" s="55">
-        <v>45989</v>
+        <v>45993</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="C24" t="s">
         <v>27</v>
@@ -1740,16 +1740,16 @@
         <v>10</v>
       </c>
       <c r="E24">
-        <v>402.29500000000002</v>
+        <v>411.5</v>
       </c>
       <c r="F24">
-        <v>4043.05</v>
+        <v>4135.6000000000004</v>
       </c>
       <c r="G24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I24">
-        <v>20.100000000000001</v>
+        <v>20.6</v>
       </c>
       <c r="J24">
         <f>Index!$C$2</f>
@@ -1758,7 +1758,7 @@
     </row>
     <row r="25" spans="1:10" ht="13" customHeight="1">
       <c r="A25" s="55">
-        <v>45988</v>
+        <v>45989</v>
       </c>
       <c r="B25" t="s">
         <v>26</v>
@@ -1770,16 +1770,16 @@
         <v>10</v>
       </c>
       <c r="E25">
-        <v>405.75</v>
+        <v>402.29500000000002</v>
       </c>
       <c r="F25">
-        <v>4077.8</v>
+        <v>4043.05</v>
       </c>
       <c r="G25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I25">
-        <v>20.3</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="J25">
         <f>Index!$C$2</f>
@@ -1788,28 +1788,28 @@
     </row>
     <row r="26" spans="1:10" ht="13" customHeight="1">
       <c r="A26" s="55">
-        <v>45982</v>
+        <v>45988</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="C26" t="s">
         <v>27</v>
       </c>
       <c r="D26">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E26">
-        <v>395.7</v>
+        <v>405.75</v>
       </c>
       <c r="F26">
-        <v>7953.6</v>
+        <v>4077.8</v>
       </c>
       <c r="G26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I26">
-        <v>39.6</v>
+        <v>20.3</v>
       </c>
       <c r="J26">
         <f>Index!$C$2</f>
@@ -1818,10 +1818,10 @@
     </row>
     <row r="27" spans="1:10" ht="13" customHeight="1">
       <c r="A27" s="55">
-        <v>45981</v>
+        <v>45982</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="C27" t="s">
         <v>27</v>
@@ -1830,16 +1830,16 @@
         <v>20</v>
       </c>
       <c r="E27">
-        <v>400.85</v>
+        <v>395.7</v>
       </c>
       <c r="F27">
-        <v>8057</v>
+        <v>7953.6</v>
       </c>
       <c r="G27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I27">
-        <v>40</v>
+        <v>39.6</v>
       </c>
       <c r="J27">
         <f>Index!$C$2</f>
@@ -1848,7 +1848,7 @@
     </row>
     <row r="28" spans="1:10" ht="13" customHeight="1">
       <c r="A28" s="55">
-        <v>45978</v>
+        <v>45981</v>
       </c>
       <c r="B28" t="s">
         <v>26</v>
@@ -1860,16 +1860,16 @@
         <v>20</v>
       </c>
       <c r="E28">
-        <v>408</v>
+        <v>400.85</v>
       </c>
       <c r="F28">
-        <v>8200.7999999999993</v>
+        <v>8057</v>
       </c>
       <c r="G28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I28">
-        <v>40.799999999999997</v>
+        <v>40</v>
       </c>
       <c r="J28">
         <f>Index!$C$2</f>
@@ -1878,7 +1878,7 @@
     </row>
     <row r="29" spans="1:10" ht="13" customHeight="1">
       <c r="A29" s="55">
-        <v>45975</v>
+        <v>45978</v>
       </c>
       <c r="B29" t="s">
         <v>26</v>
@@ -1887,19 +1887,19 @@
         <v>27</v>
       </c>
       <c r="D29">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E29">
-        <v>408.1</v>
+        <v>408</v>
       </c>
       <c r="F29">
-        <v>4101.3999999999996</v>
+        <v>8200.7999999999993</v>
       </c>
       <c r="G29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I29">
-        <v>20.399999999999999</v>
+        <v>40.799999999999997</v>
       </c>
       <c r="J29">
         <f>Index!$C$2</f>
@@ -1908,7 +1908,7 @@
     </row>
     <row r="30" spans="1:10" ht="13" customHeight="1">
       <c r="A30" s="55">
-        <v>45974</v>
+        <v>45975</v>
       </c>
       <c r="B30" t="s">
         <v>26</v>
@@ -1917,19 +1917,19 @@
         <v>27</v>
       </c>
       <c r="D30">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E30">
-        <v>410.45</v>
+        <v>408.1</v>
       </c>
       <c r="F30">
-        <v>8250</v>
+        <v>4101.3999999999996</v>
       </c>
       <c r="G30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I30">
-        <v>41</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="J30">
         <f>Index!$C$2</f>
@@ -1938,7 +1938,7 @@
     </row>
     <row r="31" spans="1:10" ht="13" customHeight="1">
       <c r="A31" s="55">
-        <v>45972</v>
+        <v>45974</v>
       </c>
       <c r="B31" t="s">
         <v>26</v>
@@ -1947,19 +1947,19 @@
         <v>27</v>
       </c>
       <c r="D31">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E31">
-        <v>414.85</v>
+        <v>410.45</v>
       </c>
       <c r="F31">
-        <v>4169.2</v>
+        <v>8250</v>
       </c>
       <c r="G31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I31">
-        <v>20.7</v>
+        <v>41</v>
       </c>
       <c r="J31">
         <f>Index!$C$2</f>
@@ -1968,7 +1968,7 @@
     </row>
     <row r="32" spans="1:10" ht="13" customHeight="1">
       <c r="A32" s="55">
-        <v>45959</v>
+        <v>45972</v>
       </c>
       <c r="B32" t="s">
         <v>26</v>
@@ -1980,16 +1980,16 @@
         <v>10</v>
       </c>
       <c r="E32">
-        <v>454.75</v>
+        <v>414.85</v>
       </c>
       <c r="F32">
-        <v>4570.2</v>
+        <v>4169.2</v>
       </c>
       <c r="G32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I32">
-        <v>22.7</v>
+        <v>20.7</v>
       </c>
       <c r="J32">
         <f>Index!$C$2</f>
@@ -1998,7 +1998,7 @@
     </row>
     <row r="33" spans="1:30" ht="13" customHeight="1">
       <c r="A33" s="55">
-        <v>45957</v>
+        <v>45959</v>
       </c>
       <c r="B33" t="s">
         <v>26</v>
@@ -2010,16 +2010,16 @@
         <v>10</v>
       </c>
       <c r="E33">
-        <v>440.65</v>
+        <v>454.75</v>
       </c>
       <c r="F33">
-        <v>4428.5</v>
+        <v>4570.2</v>
       </c>
       <c r="G33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I33">
-        <v>22</v>
+        <v>22.7</v>
       </c>
       <c r="J33">
         <f>Index!$C$2</f>
@@ -2027,96 +2027,34 @@
       </c>
     </row>
     <row r="34" spans="1:30" ht="13" customHeight="1">
-      <c r="A34" s="25">
-        <v>45954</v>
-      </c>
-      <c r="B34" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="C34" s="26" t="s">
+      <c r="A34" s="55">
+        <v>45957</v>
+      </c>
+      <c r="B34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" t="s">
         <v>27</v>
       </c>
-      <c r="D34" s="27">
-        <v>3</v>
-      </c>
-      <c r="E34" s="28">
-        <v>447.35</v>
-      </c>
-      <c r="F34" s="28">
-        <v>8450.59</v>
-      </c>
-      <c r="G34" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="H34" s="27">
-        <v>8.39</v>
-      </c>
-      <c r="I34" s="27"/>
-      <c r="J34" s="29">
+      <c r="D34">
+        <v>10</v>
+      </c>
+      <c r="E34">
+        <v>440.65</v>
+      </c>
+      <c r="F34">
+        <v>4428.5</v>
+      </c>
+      <c r="G34" t="s">
+        <v>57</v>
+      </c>
+      <c r="I34">
+        <v>22</v>
+      </c>
+      <c r="J34">
         <f>Index!$C$2</f>
         <v>338.15</v>
       </c>
-      <c r="K34" s="30" t="e">
-        <f>IF(AND(#REF!= "Buy", ISBLANK(#REF!),#REF!&lt;&gt; "DIV"),#REF!/ SUM(#REF!), "")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L34" s="31" t="e">
-        <f>IF(AND(#REF!= "Buy", ISBLANK(#REF!),#REF!&lt;&gt; "DIV"), (1-Index!$F$2*2)*((#REF!*#REF!)-(#REF!*#REF!)), "")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M34" s="31" t="e">
-        <f>IF(AND(#REF!= "Buy", ISBLANK(#REF!),#REF!&lt;&gt; "DIV"), ((#REF!*#REF!)+#REF!), "")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N34" s="32" t="e">
-        <f>IF(AND(#REF!= "Buy", ISBLANK(#REF!),#REF!&lt;&gt; "DIV"),#REF!, "")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O34" s="30" t="e">
-        <f ca="1">IF(AND(#REF!= "Buy", ISBLANK(#REF!),#REF!&lt;&gt; "DIV", NOW()-#REF! &lt; 365),#REF!/ SUM(#REF!), "")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P34" s="31" t="e">
-        <f ca="1">IF(AND(#REF!= "Buy", ISBLANK(#REF!),#REF!&lt;&gt; "DIV", NOW()-#REF! &lt; 365), (1-Index!$F$2*2)*((#REF!*#REF!)-(#REF!*#REF!)), "")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q34" s="31" t="e">
-        <f ca="1">IF(AND(#REF!= "Buy", ISBLANK(#REF!),#REF!&lt;&gt; "DIV", NOW()-#REF! &lt; 365), ((#REF!*#REF!)+#REF!), "")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="R34" s="31" t="e">
-        <f ca="1">IF(AND(#REF!= "Buy", ISBLANK(#REF!),#REF!&lt;&gt; "DIV", NOW()-#REF! &lt; 365),#REF!, "")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="S34" s="33" t="e">
-        <f ca="1">IF(AND(#REF!= "Buy", ISBLANK(#REF!),#REF!&lt;&gt; "DIV", NOW()-#REF! &gt; 365),#REF!/ SUM(#REF!), "")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="T34" s="34" t="e">
-        <f ca="1">IF(AND(#REF!= "Buy", ISBLANK(#REF!),#REF!&lt;&gt; "DIV", NOW()-#REF! &gt; 365), (1-Index!$F$2*2)*((#REF!*#REF!)-(#REF!*#REF!)), "")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="U34" s="34" t="e">
-        <f ca="1">IF(AND(#REF!= "Buy", ISBLANK(#REF!),#REF!&lt;&gt; "DIV", NOW()-#REF! &gt; 365), ((#REF!*#REF!)+#REF!), "")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="V34" s="34" t="e">
-        <f ca="1">IF(AND(#REF!= "Buy", ISBLANK(#REF!),#REF!&lt;&gt; "DIV", NOW()-#REF! &gt; 365),#REF!, "")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="W34" s="34"/>
-      <c r="X34" s="34"/>
-      <c r="Y34" s="33" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="Z34" s="34"/>
-      <c r="AA34" s="34"/>
-      <c r="AB34" s="35"/>
-      <c r="AC34" s="31" t="e">
-        <f>IF(#REF!="DIV",#REF!, "")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AD34" s="36"/>
     </row>
     <row r="35" spans="1:30" ht="13" customHeight="1">
       <c r="A35" s="25">
@@ -2129,7 +2067,7 @@
         <v>27</v>
       </c>
       <c r="D35" s="27">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E35" s="28">
         <v>447.35</v>
@@ -2212,7 +2150,7 @@
     </row>
     <row r="36" spans="1:30" ht="13" customHeight="1">
       <c r="A36" s="25">
-        <v>45950</v>
+        <v>45954</v>
       </c>
       <c r="B36" s="26" t="s">
         <v>45</v>
@@ -2221,7 +2159,7 @@
         <v>27</v>
       </c>
       <c r="D36" s="27">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E36" s="28">
         <v>447.35</v>
@@ -2304,7 +2242,7 @@
     </row>
     <row r="37" spans="1:30" ht="13" customHeight="1">
       <c r="A37" s="25">
-        <v>45947</v>
+        <v>45950</v>
       </c>
       <c r="B37" s="26" t="s">
         <v>45</v>
@@ -2313,10 +2251,10 @@
         <v>27</v>
       </c>
       <c r="D37" s="27">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E37" s="28">
-        <v>455.15</v>
+        <v>447.35</v>
       </c>
       <c r="F37" s="28">
         <v>8450.59</v>
@@ -2396,32 +2334,30 @@
     </row>
     <row r="38" spans="1:30" ht="13" customHeight="1">
       <c r="A38" s="25">
-        <v>45856</v>
+        <v>45947</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="C38" s="26" t="s">
         <v>27</v>
       </c>
       <c r="D38" s="27">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E38" s="28">
-        <v>2.5</v>
+        <v>455.15</v>
       </c>
       <c r="F38" s="28">
-        <v>50</v>
+        <v>8450.59</v>
       </c>
       <c r="G38" s="26" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H38" s="27">
-        <v>0</v>
-      </c>
-      <c r="I38" s="27">
-        <v>0</v>
-      </c>
+        <v>8.39</v>
+      </c>
+      <c r="I38" s="27"/>
       <c r="J38" s="29">
         <f>Index!$C$2</f>
         <v>338.15</v>
@@ -2499,13 +2435,13 @@
         <v>27</v>
       </c>
       <c r="D39" s="27">
-        <v>107</v>
+        <v>20</v>
       </c>
       <c r="E39" s="28">
         <v>2.5</v>
       </c>
       <c r="F39" s="28">
-        <v>267.5</v>
+        <v>50</v>
       </c>
       <c r="G39" s="26" t="s">
         <v>58</v>
@@ -2584,30 +2520,32 @@
     </row>
     <row r="40" spans="1:30" ht="13" customHeight="1">
       <c r="A40" s="25">
-        <v>45855</v>
+        <v>45856</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="C40" s="26" t="s">
         <v>27</v>
       </c>
       <c r="D40" s="27">
-        <v>20</v>
+        <v>107</v>
       </c>
       <c r="E40" s="28">
-        <v>422.53</v>
+        <v>2.5</v>
       </c>
       <c r="F40" s="28">
-        <v>8450.59</v>
+        <v>267.5</v>
       </c>
       <c r="G40" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H40" s="27">
-        <v>8.39</v>
-      </c>
-      <c r="I40" s="27"/>
+        <v>0</v>
+      </c>
+      <c r="I40" s="27">
+        <v>0</v>
+      </c>
       <c r="J40" s="29">
         <f>Index!$C$2</f>
         <v>338.15</v>
@@ -2676,28 +2614,28 @@
     </row>
     <row r="41" spans="1:30" ht="13" customHeight="1">
       <c r="A41" s="25">
-        <v>45849</v>
+        <v>45855</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="C41" s="26" t="s">
         <v>27</v>
       </c>
       <c r="D41" s="27">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="E41" s="28">
-        <v>424.44</v>
+        <v>422.53</v>
       </c>
       <c r="F41" s="28">
-        <v>16128.6</v>
+        <v>8450.59</v>
       </c>
       <c r="G41" s="26" t="s">
         <v>59</v>
       </c>
       <c r="H41" s="27">
-        <v>15.98</v>
+        <v>8.39</v>
       </c>
       <c r="I41" s="27"/>
       <c r="J41" s="29">
@@ -2777,19 +2715,19 @@
         <v>27</v>
       </c>
       <c r="D42" s="27">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="E42" s="28">
         <v>424.44</v>
       </c>
       <c r="F42" s="28">
-        <v>848.88</v>
+        <v>16128.6</v>
       </c>
       <c r="G42" s="26" t="s">
         <v>59</v>
       </c>
       <c r="H42" s="27">
-        <v>0.84</v>
+        <v>15.98</v>
       </c>
       <c r="I42" s="27"/>
       <c r="J42" s="29">
@@ -2860,7 +2798,7 @@
     </row>
     <row r="43" spans="1:30" ht="13" customHeight="1">
       <c r="A43" s="25">
-        <v>45842</v>
+        <v>45849</v>
       </c>
       <c r="B43" s="26" t="s">
         <v>26</v>
@@ -2869,19 +2807,19 @@
         <v>27</v>
       </c>
       <c r="D43" s="27">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="E43" s="28">
-        <v>435.86</v>
+        <v>424.44</v>
       </c>
       <c r="F43" s="28">
-        <v>11332.31</v>
+        <v>848.88</v>
       </c>
       <c r="G43" s="26" t="s">
         <v>59</v>
       </c>
       <c r="H43" s="27">
-        <v>11.23</v>
+        <v>0.84</v>
       </c>
       <c r="I43" s="27"/>
       <c r="J43" s="29">
@@ -2961,19 +2899,19 @@
         <v>27</v>
       </c>
       <c r="D44" s="27">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="E44" s="28">
-        <v>435.81</v>
+        <v>435.86</v>
       </c>
       <c r="F44" s="28">
-        <v>871.62</v>
+        <v>11332.31</v>
       </c>
       <c r="G44" s="26" t="s">
         <v>59</v>
       </c>
       <c r="H44" s="27">
-        <v>0.87</v>
+        <v>11.23</v>
       </c>
       <c r="I44" s="27"/>
       <c r="J44" s="29">
@@ -3136,7 +3074,7 @@
     </row>
     <row r="46" spans="1:30" ht="13" customHeight="1">
       <c r="A46" s="25">
-        <v>45821</v>
+        <v>45842</v>
       </c>
       <c r="B46" s="26" t="s">
         <v>26</v>
@@ -3145,19 +3083,19 @@
         <v>27</v>
       </c>
       <c r="D46" s="27">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E46" s="28">
-        <v>441.31</v>
+        <v>435.81</v>
       </c>
       <c r="F46" s="28">
-        <v>3089.19</v>
+        <v>871.62</v>
       </c>
       <c r="G46" s="26" t="s">
         <v>59</v>
       </c>
       <c r="H46" s="27">
-        <v>3.08</v>
+        <v>0.87</v>
       </c>
       <c r="I46" s="27"/>
       <c r="J46" s="29">
@@ -3228,7 +3166,7 @@
     </row>
     <row r="47" spans="1:30" ht="13" customHeight="1">
       <c r="A47" s="25">
-        <v>45820</v>
+        <v>45821</v>
       </c>
       <c r="B47" s="26" t="s">
         <v>26</v>
@@ -3237,19 +3175,19 @@
         <v>27</v>
       </c>
       <c r="D47" s="27">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="E47" s="28">
-        <v>454.8</v>
+        <v>441.31</v>
       </c>
       <c r="F47" s="28">
-        <v>11370.03</v>
+        <v>3089.19</v>
       </c>
       <c r="G47" s="26" t="s">
         <v>59</v>
       </c>
       <c r="H47" s="27">
-        <v>11.27</v>
+        <v>3.08</v>
       </c>
       <c r="I47" s="27"/>
       <c r="J47" s="29">
@@ -3329,19 +3267,19 @@
         <v>27</v>
       </c>
       <c r="D48" s="27">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E48" s="28">
         <v>454.8</v>
       </c>
       <c r="F48" s="28">
-        <v>2274.02</v>
+        <v>11370.03</v>
       </c>
       <c r="G48" s="26" t="s">
         <v>59</v>
       </c>
       <c r="H48" s="27">
-        <v>2.2599999999999998</v>
+        <v>11.27</v>
       </c>
       <c r="I48" s="27"/>
       <c r="J48" s="29">
@@ -3410,23 +3348,99 @@
       </c>
       <c r="AD48" s="36"/>
     </row>
-    <row r="49" spans="5:29" ht="13" customHeight="1">
-      <c r="E49" s="37"/>
-      <c r="F49" s="37"/>
-      <c r="G49" s="38"/>
-      <c r="J49" s="37"/>
-      <c r="K49" s="37"/>
-      <c r="L49" s="37"/>
-      <c r="M49" s="1"/>
-      <c r="W49" s="37"/>
-      <c r="X49" s="37"/>
-      <c r="Y49" s="37"/>
-      <c r="Z49" s="37"/>
-      <c r="AA49" s="37"/>
-      <c r="AB49" s="37"/>
-      <c r="AC49" s="37"/>
-    </row>
-    <row r="50" spans="5:29" ht="13" customHeight="1">
+    <row r="49" spans="1:30" ht="13" customHeight="1">
+      <c r="A49" s="25">
+        <v>45820</v>
+      </c>
+      <c r="B49" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D49" s="27">
+        <v>5</v>
+      </c>
+      <c r="E49" s="28">
+        <v>454.8</v>
+      </c>
+      <c r="F49" s="28">
+        <v>2274.02</v>
+      </c>
+      <c r="G49" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="H49" s="27">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="I49" s="27"/>
+      <c r="J49" s="29">
+        <f>Index!$C$2</f>
+        <v>338.15</v>
+      </c>
+      <c r="K49" s="30" t="e">
+        <f>IF(AND(#REF!= "Buy", ISBLANK(#REF!),#REF!&lt;&gt; "DIV"),#REF!/ SUM(#REF!), "")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L49" s="31" t="e">
+        <f>IF(AND(#REF!= "Buy", ISBLANK(#REF!),#REF!&lt;&gt; "DIV"), (1-Index!$F$2*2)*((#REF!*#REF!)-(#REF!*#REF!)), "")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M49" s="31" t="e">
+        <f>IF(AND(#REF!= "Buy", ISBLANK(#REF!),#REF!&lt;&gt; "DIV"), ((#REF!*#REF!)+#REF!), "")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="N49" s="32" t="e">
+        <f>IF(AND(#REF!= "Buy", ISBLANK(#REF!),#REF!&lt;&gt; "DIV"),#REF!, "")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O49" s="30" t="e">
+        <f ca="1">IF(AND(#REF!= "Buy", ISBLANK(#REF!),#REF!&lt;&gt; "DIV", NOW()-#REF! &lt; 365),#REF!/ SUM(#REF!), "")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="P49" s="31" t="e">
+        <f ca="1">IF(AND(#REF!= "Buy", ISBLANK(#REF!),#REF!&lt;&gt; "DIV", NOW()-#REF! &lt; 365), (1-Index!$F$2*2)*((#REF!*#REF!)-(#REF!*#REF!)), "")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q49" s="31" t="e">
+        <f ca="1">IF(AND(#REF!= "Buy", ISBLANK(#REF!),#REF!&lt;&gt; "DIV", NOW()-#REF! &lt; 365), ((#REF!*#REF!)+#REF!), "")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R49" s="31" t="e">
+        <f ca="1">IF(AND(#REF!= "Buy", ISBLANK(#REF!),#REF!&lt;&gt; "DIV", NOW()-#REF! &lt; 365),#REF!, "")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S49" s="33" t="e">
+        <f ca="1">IF(AND(#REF!= "Buy", ISBLANK(#REF!),#REF!&lt;&gt; "DIV", NOW()-#REF! &gt; 365),#REF!/ SUM(#REF!), "")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="T49" s="34" t="e">
+        <f ca="1">IF(AND(#REF!= "Buy", ISBLANK(#REF!),#REF!&lt;&gt; "DIV", NOW()-#REF! &gt; 365), (1-Index!$F$2*2)*((#REF!*#REF!)-(#REF!*#REF!)), "")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="U49" s="34" t="e">
+        <f ca="1">IF(AND(#REF!= "Buy", ISBLANK(#REF!),#REF!&lt;&gt; "DIV", NOW()-#REF! &gt; 365), ((#REF!*#REF!)+#REF!), "")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="V49" s="34" t="e">
+        <f ca="1">IF(AND(#REF!= "Buy", ISBLANK(#REF!),#REF!&lt;&gt; "DIV", NOW()-#REF! &gt; 365),#REF!, "")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="W49" s="34"/>
+      <c r="X49" s="34"/>
+      <c r="Y49" s="33" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="Z49" s="34"/>
+      <c r="AA49" s="34"/>
+      <c r="AB49" s="35"/>
+      <c r="AC49" s="31" t="e">
+        <f>IF(#REF!="DIV",#REF!, "")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AD49" s="36"/>
+    </row>
+    <row r="50" spans="1:30" ht="13" customHeight="1">
       <c r="E50" s="37"/>
       <c r="F50" s="37"/>
       <c r="G50" s="38"/>
@@ -3442,7 +3456,7 @@
       <c r="AB50" s="37"/>
       <c r="AC50" s="37"/>
     </row>
-    <row r="51" spans="5:29" ht="13" customHeight="1">
+    <row r="51" spans="1:30" ht="13" customHeight="1">
       <c r="E51" s="37"/>
       <c r="F51" s="37"/>
       <c r="G51" s="38"/>
@@ -3458,7 +3472,7 @@
       <c r="AB51" s="37"/>
       <c r="AC51" s="37"/>
     </row>
-    <row r="52" spans="5:29" ht="13" customHeight="1">
+    <row r="52" spans="1:30" ht="13" customHeight="1">
       <c r="E52" s="37"/>
       <c r="F52" s="37"/>
       <c r="G52" s="38"/>
@@ -3474,7 +3488,7 @@
       <c r="AB52" s="37"/>
       <c r="AC52" s="37"/>
     </row>
-    <row r="53" spans="5:29" ht="13" customHeight="1">
+    <row r="53" spans="1:30" ht="13" customHeight="1">
       <c r="E53" s="37"/>
       <c r="F53" s="37"/>
       <c r="G53" s="38"/>
@@ -3490,7 +3504,7 @@
       <c r="AB53" s="37"/>
       <c r="AC53" s="37"/>
     </row>
-    <row r="54" spans="5:29" ht="13" customHeight="1">
+    <row r="54" spans="1:30" ht="13" customHeight="1">
       <c r="E54" s="37"/>
       <c r="F54" s="37"/>
       <c r="G54" s="38"/>
@@ -3506,7 +3520,7 @@
       <c r="AB54" s="37"/>
       <c r="AC54" s="37"/>
     </row>
-    <row r="55" spans="5:29" ht="13" customHeight="1">
+    <row r="55" spans="1:30" ht="13" customHeight="1">
       <c r="E55" s="37"/>
       <c r="F55" s="37"/>
       <c r="G55" s="38"/>
@@ -3522,7 +3536,7 @@
       <c r="AB55" s="37"/>
       <c r="AC55" s="37"/>
     </row>
-    <row r="56" spans="5:29" ht="13" customHeight="1">
+    <row r="56" spans="1:30" ht="13" customHeight="1">
       <c r="E56" s="37"/>
       <c r="F56" s="37"/>
       <c r="G56" s="38"/>
@@ -3538,7 +3552,7 @@
       <c r="AB56" s="37"/>
       <c r="AC56" s="37"/>
     </row>
-    <row r="57" spans="5:29" ht="13" customHeight="1">
+    <row r="57" spans="1:30" ht="13" customHeight="1">
       <c r="E57" s="37"/>
       <c r="F57" s="37"/>
       <c r="G57" s="38"/>
@@ -3554,7 +3568,7 @@
       <c r="AB57" s="37"/>
       <c r="AC57" s="37"/>
     </row>
-    <row r="58" spans="5:29" ht="13" customHeight="1">
+    <row r="58" spans="1:30" ht="13" customHeight="1">
       <c r="E58" s="37"/>
       <c r="F58" s="37"/>
       <c r="G58" s="38"/>
@@ -3570,7 +3584,7 @@
       <c r="AB58" s="37"/>
       <c r="AC58" s="37"/>
     </row>
-    <row r="59" spans="5:29" ht="13" customHeight="1">
+    <row r="59" spans="1:30" ht="13" customHeight="1">
       <c r="E59" s="37"/>
       <c r="F59" s="37"/>
       <c r="G59" s="38"/>
@@ -3586,7 +3600,7 @@
       <c r="AB59" s="37"/>
       <c r="AC59" s="37"/>
     </row>
-    <row r="60" spans="5:29" ht="13" customHeight="1">
+    <row r="60" spans="1:30" ht="13" customHeight="1">
       <c r="E60" s="37"/>
       <c r="F60" s="37"/>
       <c r="G60" s="38"/>
@@ -3602,7 +3616,7 @@
       <c r="AB60" s="37"/>
       <c r="AC60" s="37"/>
     </row>
-    <row r="61" spans="5:29" ht="13" customHeight="1">
+    <row r="61" spans="1:30" ht="13" customHeight="1">
       <c r="E61" s="37"/>
       <c r="F61" s="37"/>
       <c r="G61" s="38"/>
@@ -3618,7 +3632,7 @@
       <c r="AB61" s="37"/>
       <c r="AC61" s="37"/>
     </row>
-    <row r="62" spans="5:29" ht="13" customHeight="1">
+    <row r="62" spans="1:30" ht="13" customHeight="1">
       <c r="E62" s="37"/>
       <c r="F62" s="37"/>
       <c r="G62" s="38"/>
@@ -3634,7 +3648,7 @@
       <c r="AB62" s="37"/>
       <c r="AC62" s="37"/>
     </row>
-    <row r="63" spans="5:29" ht="13" customHeight="1">
+    <row r="63" spans="1:30" ht="13" customHeight="1">
       <c r="E63" s="37"/>
       <c r="F63" s="37"/>
       <c r="G63" s="38"/>
@@ -3650,7 +3664,7 @@
       <c r="AB63" s="37"/>
       <c r="AC63" s="37"/>
     </row>
-    <row r="64" spans="5:29" ht="13" customHeight="1">
+    <row r="64" spans="1:30" ht="13" customHeight="1">
       <c r="E64" s="37"/>
       <c r="F64" s="37"/>
       <c r="G64" s="38"/>
@@ -18194,7 +18208,7 @@
       <c r="AB972" s="37"/>
       <c r="AC972" s="37"/>
     </row>
-    <row r="973" spans="5:29" ht="13">
+    <row r="973" spans="5:29" ht="13" customHeight="1">
       <c r="E973" s="37"/>
       <c r="F973" s="37"/>
       <c r="G973" s="38"/>
@@ -18393,6 +18407,7 @@
       <c r="J985" s="37"/>
       <c r="K985" s="37"/>
       <c r="L985" s="37"/>
+      <c r="M985" s="1"/>
       <c r="W985" s="37"/>
       <c r="X985" s="37"/>
       <c r="Y985" s="37"/>
@@ -18641,6 +18656,21 @@
       <c r="AB1001" s="37"/>
       <c r="AC1001" s="37"/>
     </row>
+    <row r="1002" spans="5:29" ht="13">
+      <c r="E1002" s="37"/>
+      <c r="F1002" s="37"/>
+      <c r="G1002" s="38"/>
+      <c r="J1002" s="37"/>
+      <c r="K1002" s="37"/>
+      <c r="L1002" s="37"/>
+      <c r="W1002" s="37"/>
+      <c r="X1002" s="37"/>
+      <c r="Y1002" s="37"/>
+      <c r="Z1002" s="37"/>
+      <c r="AA1002" s="37"/>
+      <c r="AB1002" s="37"/>
+      <c r="AC1002" s="37"/>
+    </row>
   </sheetData>
   <autoFilter ref="A4:AO4" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="5">
@@ -18650,12 +18680,12 @@
     <mergeCell ref="K3:N3"/>
     <mergeCell ref="O3:R3"/>
   </mergeCells>
-  <conditionalFormatting sqref="B1:B2 B4:B923">
+  <conditionalFormatting sqref="B1:B2 B4:B924">
     <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="DIV">
       <formula>NOT(ISERROR(SEARCH(("DIV"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C923">
+  <conditionalFormatting sqref="C1:C924">
     <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Buy">
       <formula>NOT(ISERROR(SEARCH(("Buy"),(C1))))</formula>
     </cfRule>
@@ -18900,7 +18930,7 @@
         <v>18</v>
       </c>
       <c r="C8" s="45" t="e">
-        <f>SUM('Trading History'!$N$4:$N961)</f>
+        <f>SUM('Trading History'!$N$4:$N962)</f>
         <v>#REF!</v>
       </c>
       <c r="D8" s="42"/>
@@ -18908,7 +18938,7 @@
         <v>66</v>
       </c>
       <c r="F8" s="45">
-        <f ca="1">IFERROR(SUM('Trading History'!$R$4:$R961), 0)</f>
+        <f ca="1">IFERROR(SUM('Trading History'!$R$4:$R962), 0)</f>
         <v>0</v>
       </c>
       <c r="G8" s="42"/>
@@ -18916,7 +18946,7 @@
         <v>67</v>
       </c>
       <c r="I8" s="45" t="e">
-        <f ca="1">SUM('Trading History'!$V$4:$V961)</f>
+        <f ca="1">SUM('Trading History'!$V$4:$V962)</f>
         <v>#REF!</v>
       </c>
       <c r="J8" s="42"/>
@@ -18924,7 +18954,7 @@
         <v>18</v>
       </c>
       <c r="L8" s="45">
-        <f>SUM('Trading History'!$AB$4:$AB961)</f>
+        <f>SUM('Trading History'!$AB$4:$AB962)</f>
         <v>0</v>
       </c>
       <c r="M8" s="1"/>
@@ -18994,7 +19024,7 @@
         <v>16</v>
       </c>
       <c r="C10" s="53" t="e">
-        <f>SUM('Trading History'!$L$4:$L961)</f>
+        <f>SUM('Trading History'!$L$4:$L962)</f>
         <v>#REF!</v>
       </c>
       <c r="D10" s="42"/>
@@ -19002,7 +19032,7 @@
         <v>71</v>
       </c>
       <c r="F10" s="53" t="e">
-        <f ca="1">SUM('Trading History'!$P$4:$P961)</f>
+        <f ca="1">SUM('Trading History'!$P$4:$P962)</f>
         <v>#REF!</v>
       </c>
       <c r="G10" s="42"/>
@@ -19010,7 +19040,7 @@
         <v>72</v>
       </c>
       <c r="I10" s="53" t="e">
-        <f ca="1">SUM('Trading History'!$T$4:$T961)</f>
+        <f ca="1">SUM('Trading History'!$T$4:$T962)</f>
         <v>#REF!</v>
       </c>
       <c r="J10" s="42"/>
@@ -19018,7 +19048,7 @@
         <v>16</v>
       </c>
       <c r="L10" s="53">
-        <f>SUM('Trading History'!$Z$4:$Z961)</f>
+        <f>SUM('Trading History'!$Z$4:$Z962)</f>
         <v>0</v>
       </c>
       <c r="M10" s="1"/>
@@ -19088,7 +19118,7 @@
         <v>17</v>
       </c>
       <c r="C12" s="53" t="e">
-        <f>SUM('Trading History'!$M$4:$M961)</f>
+        <f>SUM('Trading History'!$M$4:$M962)</f>
         <v>#REF!</v>
       </c>
       <c r="D12" s="42"/>
@@ -19096,7 +19126,7 @@
         <v>76</v>
       </c>
       <c r="F12" s="53" t="e">
-        <f ca="1">SUM('Trading History'!$Q$4:$Q961)</f>
+        <f ca="1">SUM('Trading History'!$Q$4:$Q962)</f>
         <v>#REF!</v>
       </c>
       <c r="G12" s="42"/>
@@ -19104,7 +19134,7 @@
         <v>77</v>
       </c>
       <c r="I12" s="53" t="e">
-        <f ca="1">SUM('Trading History'!$U$4:$U961)</f>
+        <f ca="1">SUM('Trading History'!$U$4:$U962)</f>
         <v>#REF!</v>
       </c>
       <c r="J12" s="42"/>
@@ -19112,7 +19142,7 @@
         <v>17</v>
       </c>
       <c r="L12" s="53">
-        <f>SUM('Trading History'!$AA$4:$AA961)</f>
+        <f>SUM('Trading History'!$AA$4:$AA962)</f>
         <v>0</v>
       </c>
       <c r="M12" s="1"/>
@@ -19144,7 +19174,7 @@
         <v>78</v>
       </c>
       <c r="L13" s="53" t="e">
-        <f>SUMIF('Trading History'!$B5:$B961,"DIV",'Trading History'!$AC$4:$AC961)</f>
+        <f>SUMIF('Trading History'!$B5:$B962,"DIV",'Trading History'!$AC$4:$AC962)</f>
         <v>#REF!</v>
       </c>
     </row>
@@ -19170,7 +19200,7 @@
         <v>18</v>
       </c>
       <c r="C15" s="45">
-        <f ca="1">SUMIFS('Trading History'!$N$4:$N961, 'Trading History'!$K$4:$K961, _xludf.CONCAT("&gt;", $A15))</f>
+        <f ca="1">SUMIFS('Trading History'!$N$4:$N962, 'Trading History'!$K$4:$K962, _xludf.CONCAT("&gt;", $A15))</f>
         <v>0</v>
       </c>
       <c r="D15" s="42"/>
@@ -19178,7 +19208,7 @@
         <v>66</v>
       </c>
       <c r="F15" s="45">
-        <f ca="1">IFERROR(SUMIFS('Trading History'!$R$4:$R961, 'Trading History'!$O$4:$O961, _xludf.CONCAT("&gt;", $A15)), 0)</f>
+        <f ca="1">IFERROR(SUMIFS('Trading History'!$R$4:$R962, 'Trading History'!$O$4:$O962, _xludf.CONCAT("&gt;", $A15)), 0)</f>
         <v>0</v>
       </c>
       <c r="G15" s="42"/>
@@ -19186,7 +19216,7 @@
         <v>67</v>
       </c>
       <c r="I15" s="45">
-        <f ca="1">SUMIFS('Trading History'!$V$4:$V961, 'Trading History'!$S$4:$S961, _xludf.CONCAT("&gt;", $A15))</f>
+        <f ca="1">SUMIFS('Trading History'!$V$4:$V962, 'Trading History'!$S$4:$S962, _xludf.CONCAT("&gt;", $A15))</f>
         <v>0</v>
       </c>
       <c r="J15" s="42"/>
@@ -19194,7 +19224,7 @@
         <v>18</v>
       </c>
       <c r="L15" s="45">
-        <f ca="1">SUMIFS('Trading History'!$AB$4:$AB961, 'Trading History'!$Y$4:$Y961, _xludf.CONCAT("&gt;", $A15))</f>
+        <f ca="1">SUMIFS('Trading History'!$AB$4:$AB962, 'Trading History'!$Y$4:$Y962, _xludf.CONCAT("&gt;", $A15))</f>
         <v>0</v>
       </c>
       <c r="M15" s="1"/>
@@ -19264,7 +19294,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="53">
-        <f ca="1">SUMIFS('Trading History'!$L$4:$L961, 'Trading History'!$K$4:$K961, _xludf.CONCAT("&gt;", $A15))</f>
+        <f ca="1">SUMIFS('Trading History'!$L$4:$L962, 'Trading History'!$K$4:$K962, _xludf.CONCAT("&gt;", $A15))</f>
         <v>0</v>
       </c>
       <c r="D17" s="42"/>
@@ -19272,7 +19302,7 @@
         <v>71</v>
       </c>
       <c r="F17" s="53">
-        <f ca="1">SUMIFS('Trading History'!$P$4:$P961, 'Trading History'!$O$4:$O961, _xludf.CONCAT("&gt;", $A15))</f>
+        <f ca="1">SUMIFS('Trading History'!$P$4:$P962, 'Trading History'!$O$4:$O962, _xludf.CONCAT("&gt;", $A15))</f>
         <v>0</v>
       </c>
       <c r="G17" s="42"/>
@@ -19280,7 +19310,7 @@
         <v>72</v>
       </c>
       <c r="I17" s="53">
-        <f ca="1">SUMIFS('Trading History'!$T$4:$T961, 'Trading History'!$S$4:$S961, _xludf.CONCAT("&gt;", $A15))</f>
+        <f ca="1">SUMIFS('Trading History'!$T$4:$T962, 'Trading History'!$S$4:$S962, _xludf.CONCAT("&gt;", $A15))</f>
         <v>0</v>
       </c>
       <c r="J17" s="42"/>
@@ -19288,7 +19318,7 @@
         <v>16</v>
       </c>
       <c r="L17" s="53">
-        <f ca="1">SUMIFS('Trading History'!$Z$4:$Z961, 'Trading History'!$Y$4:$Y961, _xludf.CONCAT("&gt;", $A15))</f>
+        <f ca="1">SUMIFS('Trading History'!$Z$4:$Z962, 'Trading History'!$Y$4:$Y962, _xludf.CONCAT("&gt;", $A15))</f>
         <v>0</v>
       </c>
       <c r="M17" s="1"/>
@@ -19358,7 +19388,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="53">
-        <f ca="1">SUMIFS('Trading History'!$M$4:$M961, 'Trading History'!$K$4:$K961, _xludf.CONCAT("&gt;", $A15))</f>
+        <f ca="1">SUMIFS('Trading History'!$M$4:$M962, 'Trading History'!$K$4:$K962, _xludf.CONCAT("&gt;", $A15))</f>
         <v>0</v>
       </c>
       <c r="D19" s="42"/>
@@ -19366,7 +19396,7 @@
         <v>76</v>
       </c>
       <c r="F19" s="53">
-        <f ca="1">SUMIFS('Trading History'!$Q$4:$Q961, 'Trading History'!$O$4:$O961, _xludf.CONCAT("&gt;", $A15))</f>
+        <f ca="1">SUMIFS('Trading History'!$Q$4:$Q962, 'Trading History'!$O$4:$O962, _xludf.CONCAT("&gt;", $A15))</f>
         <v>0</v>
       </c>
       <c r="G19" s="42"/>
@@ -19374,7 +19404,7 @@
         <v>77</v>
       </c>
       <c r="I19" s="53">
-        <f ca="1">SUMIFS('Trading History'!$U$4:$U961, 'Trading History'!$S$4:$S961, _xludf.CONCAT("&gt;", $A15))</f>
+        <f ca="1">SUMIFS('Trading History'!$U$4:$U962, 'Trading History'!$S$4:$S962, _xludf.CONCAT("&gt;", $A15))</f>
         <v>0</v>
       </c>
       <c r="J19" s="42"/>
@@ -19382,7 +19412,7 @@
         <v>17</v>
       </c>
       <c r="L19" s="53">
-        <f ca="1">SUMIFS('Trading History'!$AA$4:$AA961, 'Trading History'!$Y$4:$Y961, _xludf.CONCAT("&gt;", $A15))</f>
+        <f ca="1">SUMIFS('Trading History'!$AA$4:$AA962, 'Trading History'!$Y$4:$Y962, _xludf.CONCAT("&gt;", $A15))</f>
         <v>0</v>
       </c>
       <c r="M19" s="1"/>
@@ -19435,7 +19465,7 @@
         <v>18</v>
       </c>
       <c r="C22" s="45">
-        <f ca="1">SUMIFS('Trading History'!$N$4:$N961, 'Trading History'!$K$4:$K961, _xludf.CONCAT("&gt;", $A22))</f>
+        <f ca="1">SUMIFS('Trading History'!$N$4:$N962, 'Trading History'!$K$4:$K962, _xludf.CONCAT("&gt;", $A22))</f>
         <v>0</v>
       </c>
       <c r="D22" s="42"/>
@@ -19443,7 +19473,7 @@
         <v>66</v>
       </c>
       <c r="F22" s="45">
-        <f ca="1">IFERROR(SUMIFS('Trading History'!$R$4:$R961, 'Trading History'!$O$4:$O961, _xludf.CONCAT("&gt;", $A22)), 0)</f>
+        <f ca="1">IFERROR(SUMIFS('Trading History'!$R$4:$R962, 'Trading History'!$O$4:$O962, _xludf.CONCAT("&gt;", $A22)), 0)</f>
         <v>0</v>
       </c>
       <c r="G22" s="42"/>
@@ -19451,7 +19481,7 @@
         <v>67</v>
       </c>
       <c r="I22" s="45">
-        <f ca="1">SUMIFS('Trading History'!$V$4:$V961, 'Trading History'!$S$4:$S961, _xludf.CONCAT("&gt;", $A22))</f>
+        <f ca="1">SUMIFS('Trading History'!$V$4:$V962, 'Trading History'!$S$4:$S962, _xludf.CONCAT("&gt;", $A22))</f>
         <v>0</v>
       </c>
       <c r="J22" s="42"/>
@@ -19459,7 +19489,7 @@
         <v>18</v>
       </c>
       <c r="L22" s="45">
-        <f ca="1">SUMIFS('Trading History'!$AB$4:$AB961, 'Trading History'!$Y$4:$Y961, _xludf.CONCAT("&gt;", $A22))</f>
+        <f ca="1">SUMIFS('Trading History'!$AB$4:$AB962, 'Trading History'!$Y$4:$Y962, _xludf.CONCAT("&gt;", $A22))</f>
         <v>0</v>
       </c>
       <c r="M22" s="1"/>
@@ -19529,7 +19559,7 @@
         <v>16</v>
       </c>
       <c r="C24" s="53">
-        <f ca="1">SUMIFS('Trading History'!$L$4:$L961, 'Trading History'!$K$4:$K961, _xludf.CONCAT("&gt;", $A22))</f>
+        <f ca="1">SUMIFS('Trading History'!$L$4:$L962, 'Trading History'!$K$4:$K962, _xludf.CONCAT("&gt;", $A22))</f>
         <v>0</v>
       </c>
       <c r="D24" s="42"/>
@@ -19537,7 +19567,7 @@
         <v>71</v>
       </c>
       <c r="F24" s="53">
-        <f ca="1">SUMIFS('Trading History'!$P$4:$P961, 'Trading History'!$O$4:$O961, _xludf.CONCAT("&gt;", $A22))</f>
+        <f ca="1">SUMIFS('Trading History'!$P$4:$P962, 'Trading History'!$O$4:$O962, _xludf.CONCAT("&gt;", $A22))</f>
         <v>0</v>
       </c>
       <c r="G24" s="42"/>
@@ -19545,7 +19575,7 @@
         <v>72</v>
       </c>
       <c r="I24" s="53">
-        <f ca="1">SUMIFS('Trading History'!$T$4:$T961, 'Trading History'!$S$4:$S961, _xludf.CONCAT("&gt;", $A22))</f>
+        <f ca="1">SUMIFS('Trading History'!$T$4:$T962, 'Trading History'!$S$4:$S962, _xludf.CONCAT("&gt;", $A22))</f>
         <v>0</v>
       </c>
       <c r="J24" s="42"/>
@@ -19553,7 +19583,7 @@
         <v>16</v>
       </c>
       <c r="L24" s="53">
-        <f ca="1">SUMIFS('Trading History'!$Z$4:$Z961, 'Trading History'!$Y$4:$Y961, _xludf.CONCAT("&gt;", $A22))</f>
+        <f ca="1">SUMIFS('Trading History'!$Z$4:$Z962, 'Trading History'!$Y$4:$Y962, _xludf.CONCAT("&gt;", $A22))</f>
         <v>0</v>
       </c>
       <c r="M24" s="1"/>
@@ -19623,7 +19653,7 @@
         <v>17</v>
       </c>
       <c r="C26" s="53">
-        <f ca="1">SUMIFS('Trading History'!$M$4:$M961, 'Trading History'!$K$4:$K961, _xludf.CONCAT("&gt;", $A22))</f>
+        <f ca="1">SUMIFS('Trading History'!$M$4:$M962, 'Trading History'!$K$4:$K962, _xludf.CONCAT("&gt;", $A22))</f>
         <v>0</v>
       </c>
       <c r="D26" s="42"/>
@@ -19631,7 +19661,7 @@
         <v>76</v>
       </c>
       <c r="F26" s="53">
-        <f ca="1">SUMIFS('Trading History'!$Q$4:$Q961, 'Trading History'!$O$4:$O961, _xludf.CONCAT("&gt;", $A22))</f>
+        <f ca="1">SUMIFS('Trading History'!$Q$4:$Q962, 'Trading History'!$O$4:$O962, _xludf.CONCAT("&gt;", $A22))</f>
         <v>0</v>
       </c>
       <c r="G26" s="42"/>
@@ -19639,7 +19669,7 @@
         <v>77</v>
       </c>
       <c r="I26" s="53">
-        <f ca="1">SUMIFS('Trading History'!$U$4:$U961, 'Trading History'!$S$4:$S961, _xludf.CONCAT("&gt;", $A22))</f>
+        <f ca="1">SUMIFS('Trading History'!$U$4:$U962, 'Trading History'!$S$4:$S962, _xludf.CONCAT("&gt;", $A22))</f>
         <v>0</v>
       </c>
       <c r="J26" s="42"/>
@@ -19647,7 +19677,7 @@
         <v>17</v>
       </c>
       <c r="L26" s="53">
-        <f ca="1">SUMIFS('Trading History'!$AA$4:$AA961, 'Trading History'!$Y$4:$Y961, _xludf.CONCAT("&gt;", $A22))</f>
+        <f ca="1">SUMIFS('Trading History'!$AA$4:$AA962, 'Trading History'!$Y$4:$Y962, _xludf.CONCAT("&gt;", $A22))</f>
         <v>0</v>
       </c>
       <c r="M26" s="1"/>
@@ -19726,7 +19756,7 @@
         <v>18</v>
       </c>
       <c r="C29" s="45">
-        <f ca="1">SUMIFS('Trading History'!$N$4:$N961, 'Trading History'!$K$4:$K961, _xludf.CONCAT("&gt;", $A29))</f>
+        <f ca="1">SUMIFS('Trading History'!$N$4:$N962, 'Trading History'!$K$4:$K962, _xludf.CONCAT("&gt;", $A29))</f>
         <v>0</v>
       </c>
       <c r="D29" s="42"/>
@@ -19734,7 +19764,7 @@
         <v>66</v>
       </c>
       <c r="F29" s="45">
-        <f ca="1">IFERROR(SUMIFS('Trading History'!$R$4:$R961, 'Trading History'!$O$4:$O961, _xludf.CONCAT("&gt;", $A29)), 0)</f>
+        <f ca="1">IFERROR(SUMIFS('Trading History'!$R$4:$R962, 'Trading History'!$O$4:$O962, _xludf.CONCAT("&gt;", $A29)), 0)</f>
         <v>0</v>
       </c>
       <c r="G29" s="42"/>
@@ -19742,7 +19772,7 @@
         <v>67</v>
       </c>
       <c r="I29" s="45">
-        <f ca="1">SUMIFS('Trading History'!$V$4:$V961, 'Trading History'!$S$4:$S961, _xludf.CONCAT("&gt;", $A29))</f>
+        <f ca="1">SUMIFS('Trading History'!$V$4:$V962, 'Trading History'!$S$4:$S962, _xludf.CONCAT("&gt;", $A29))</f>
         <v>0</v>
       </c>
       <c r="J29" s="42"/>
@@ -19750,7 +19780,7 @@
         <v>18</v>
       </c>
       <c r="L29" s="45">
-        <f ca="1">SUMIFS('Trading History'!$AB$4:$AB961, 'Trading History'!$Y$4:$Y961, _xludf.CONCAT("&gt;", $A29))</f>
+        <f ca="1">SUMIFS('Trading History'!$AB$4:$AB962, 'Trading History'!$Y$4:$Y962, _xludf.CONCAT("&gt;", $A29))</f>
         <v>0</v>
       </c>
       <c r="M29" s="1"/>
@@ -19820,7 +19850,7 @@
         <v>16</v>
       </c>
       <c r="C31" s="53">
-        <f ca="1">SUMIFS('Trading History'!$L$4:$L961, 'Trading History'!$K$4:$K961, _xludf.CONCAT("&gt;", $A29))</f>
+        <f ca="1">SUMIFS('Trading History'!$L$4:$L962, 'Trading History'!$K$4:$K962, _xludf.CONCAT("&gt;", $A29))</f>
         <v>0</v>
       </c>
       <c r="D31" s="42"/>
@@ -19828,7 +19858,7 @@
         <v>71</v>
       </c>
       <c r="F31" s="53">
-        <f ca="1">SUMIFS('Trading History'!$P$4:$P961, 'Trading History'!$O$4:$O961, _xludf.CONCAT("&gt;", $A29))</f>
+        <f ca="1">SUMIFS('Trading History'!$P$4:$P962, 'Trading History'!$O$4:$O962, _xludf.CONCAT("&gt;", $A29))</f>
         <v>0</v>
       </c>
       <c r="G31" s="42"/>
@@ -19836,7 +19866,7 @@
         <v>72</v>
       </c>
       <c r="I31" s="53">
-        <f ca="1">SUMIFS('Trading History'!$T$4:$T961, 'Trading History'!$S$4:$S961, _xludf.CONCAT("&gt;", $A29))</f>
+        <f ca="1">SUMIFS('Trading History'!$T$4:$T962, 'Trading History'!$S$4:$S962, _xludf.CONCAT("&gt;", $A29))</f>
         <v>0</v>
       </c>
       <c r="J31" s="42"/>
@@ -19844,7 +19874,7 @@
         <v>16</v>
       </c>
       <c r="L31" s="53">
-        <f ca="1">SUMIFS('Trading History'!$Z$4:$Z961, 'Trading History'!$Y$4:$Y961, _xludf.CONCAT("&gt;", $A29))</f>
+        <f ca="1">SUMIFS('Trading History'!$Z$4:$Z962, 'Trading History'!$Y$4:$Y962, _xludf.CONCAT("&gt;", $A29))</f>
         <v>0</v>
       </c>
       <c r="M31" s="1"/>
@@ -19914,7 +19944,7 @@
         <v>17</v>
       </c>
       <c r="C33" s="53">
-        <f ca="1">SUMIFS('Trading History'!$M$4:$M961, 'Trading History'!$K$4:$K961, _xludf.CONCAT("&gt;", $A29))</f>
+        <f ca="1">SUMIFS('Trading History'!$M$4:$M962, 'Trading History'!$K$4:$K962, _xludf.CONCAT("&gt;", $A29))</f>
         <v>0</v>
       </c>
       <c r="D33" s="42"/>
@@ -19922,7 +19952,7 @@
         <v>76</v>
       </c>
       <c r="F33" s="53">
-        <f ca="1">SUMIFS('Trading History'!$Q$4:$Q961, 'Trading History'!$O$4:$O961, _xludf.CONCAT("&gt;", $A29))</f>
+        <f ca="1">SUMIFS('Trading History'!$Q$4:$Q962, 'Trading History'!$O$4:$O962, _xludf.CONCAT("&gt;", $A29))</f>
         <v>0</v>
       </c>
       <c r="G33" s="42"/>
@@ -19930,7 +19960,7 @@
         <v>77</v>
       </c>
       <c r="I33" s="53">
-        <f ca="1">SUMIFS('Trading History'!$U$4:$U961, 'Trading History'!$S$4:$S961, _xludf.CONCAT("&gt;", $A29))</f>
+        <f ca="1">SUMIFS('Trading History'!$U$4:$U962, 'Trading History'!$S$4:$S962, _xludf.CONCAT("&gt;", $A29))</f>
         <v>0</v>
       </c>
       <c r="J33" s="42"/>
@@ -19938,7 +19968,7 @@
         <v>17</v>
       </c>
       <c r="L33" s="53">
-        <f ca="1">SUMIFS('Trading History'!$AA$4:$AA961, 'Trading History'!$Y$4:$Y961, _xludf.CONCAT("&gt;", $A29))</f>
+        <f ca="1">SUMIFS('Trading History'!$AA$4:$AA962, 'Trading History'!$Y$4:$Y962, _xludf.CONCAT("&gt;", $A29))</f>
         <v>0</v>
       </c>
       <c r="M33" s="1"/>
@@ -20017,7 +20047,7 @@
         <v>18</v>
       </c>
       <c r="C36" s="45">
-        <f ca="1">SUMIFS('Trading History'!$N$4:$N961, 'Trading History'!$K$4:$K961, _xludf.CONCAT("&gt;", $A36))</f>
+        <f ca="1">SUMIFS('Trading History'!$N$4:$N962, 'Trading History'!$K$4:$K962, _xludf.CONCAT("&gt;", $A36))</f>
         <v>0</v>
       </c>
       <c r="D36" s="42"/>
@@ -20025,7 +20055,7 @@
         <v>66</v>
       </c>
       <c r="F36" s="45">
-        <f ca="1">IFERROR(SUMIFS('Trading History'!$R$4:$R961, 'Trading History'!$O$4:$O961, _xludf.CONCAT("&gt;", $A36)), 0)</f>
+        <f ca="1">IFERROR(SUMIFS('Trading History'!$R$4:$R962, 'Trading History'!$O$4:$O962, _xludf.CONCAT("&gt;", $A36)), 0)</f>
         <v>0</v>
       </c>
       <c r="G36" s="42"/>
@@ -20033,7 +20063,7 @@
         <v>67</v>
       </c>
       <c r="I36" s="45">
-        <f ca="1">SUMIFS('Trading History'!$V$4:$V961, 'Trading History'!$S$4:$S961, _xludf.CONCAT("&gt;", $A36))</f>
+        <f ca="1">SUMIFS('Trading History'!$V$4:$V962, 'Trading History'!$S$4:$S962, _xludf.CONCAT("&gt;", $A36))</f>
         <v>0</v>
       </c>
       <c r="J36" s="42"/>
@@ -20041,7 +20071,7 @@
         <v>18</v>
       </c>
       <c r="L36" s="45">
-        <f ca="1">SUMIFS('Trading History'!$AB$4:$AB961, 'Trading History'!$Y$4:$Y961, _xludf.CONCAT("&gt;", $A36))</f>
+        <f ca="1">SUMIFS('Trading History'!$AB$4:$AB962, 'Trading History'!$Y$4:$Y962, _xludf.CONCAT("&gt;", $A36))</f>
         <v>0</v>
       </c>
       <c r="M36" s="1"/>
@@ -20111,7 +20141,7 @@
         <v>16</v>
       </c>
       <c r="C38" s="53">
-        <f ca="1">SUMIFS('Trading History'!$L$4:$L961, 'Trading History'!$K$4:$K961, _xludf.CONCAT("&gt;", $A36))</f>
+        <f ca="1">SUMIFS('Trading History'!$L$4:$L962, 'Trading History'!$K$4:$K962, _xludf.CONCAT("&gt;", $A36))</f>
         <v>0</v>
       </c>
       <c r="D38" s="42"/>
@@ -20119,7 +20149,7 @@
         <v>71</v>
       </c>
       <c r="F38" s="53">
-        <f ca="1">SUMIFS('Trading History'!$P$4:$P961, 'Trading History'!$O$4:$O961, _xludf.CONCAT("&gt;", $A36))</f>
+        <f ca="1">SUMIFS('Trading History'!$P$4:$P962, 'Trading History'!$O$4:$O962, _xludf.CONCAT("&gt;", $A36))</f>
         <v>0</v>
       </c>
       <c r="G38" s="42"/>
@@ -20127,7 +20157,7 @@
         <v>72</v>
       </c>
       <c r="I38" s="53">
-        <f ca="1">SUMIFS('Trading History'!$T$4:$T961, 'Trading History'!$S$4:$S961, _xludf.CONCAT("&gt;", $A36))</f>
+        <f ca="1">SUMIFS('Trading History'!$T$4:$T962, 'Trading History'!$S$4:$S962, _xludf.CONCAT("&gt;", $A36))</f>
         <v>0</v>
       </c>
       <c r="J38" s="42"/>
@@ -20135,7 +20165,7 @@
         <v>16</v>
       </c>
       <c r="L38" s="53">
-        <f ca="1">SUMIFS('Trading History'!$Z$4:$Z961, 'Trading History'!$Y$4:$Y961, _xludf.CONCAT("&gt;", $A36))</f>
+        <f ca="1">SUMIFS('Trading History'!$Z$4:$Z962, 'Trading History'!$Y$4:$Y962, _xludf.CONCAT("&gt;", $A36))</f>
         <v>0</v>
       </c>
       <c r="M38" s="1"/>
@@ -20205,7 +20235,7 @@
         <v>17</v>
       </c>
       <c r="C40" s="53">
-        <f ca="1">SUMIFS('Trading History'!$M$4:$M961, 'Trading History'!$K$4:$K961, _xludf.CONCAT("&gt;", $A36))</f>
+        <f ca="1">SUMIFS('Trading History'!$M$4:$M962, 'Trading History'!$K$4:$K962, _xludf.CONCAT("&gt;", $A36))</f>
         <v>0</v>
       </c>
       <c r="D40" s="42"/>
@@ -20213,7 +20243,7 @@
         <v>76</v>
       </c>
       <c r="F40" s="53">
-        <f ca="1">SUMIFS('Trading History'!$Q$4:$Q961, 'Trading History'!$O$4:$O961, _xludf.CONCAT("&gt;", $A36))</f>
+        <f ca="1">SUMIFS('Trading History'!$Q$4:$Q962, 'Trading History'!$O$4:$O962, _xludf.CONCAT("&gt;", $A36))</f>
         <v>0</v>
       </c>
       <c r="G40" s="42"/>
@@ -20221,7 +20251,7 @@
         <v>77</v>
       </c>
       <c r="I40" s="53">
-        <f ca="1">SUMIFS('Trading History'!$U$4:$U961, 'Trading History'!$S$4:$S961, _xludf.CONCAT("&gt;", $A36))</f>
+        <f ca="1">SUMIFS('Trading History'!$U$4:$U962, 'Trading History'!$S$4:$S962, _xludf.CONCAT("&gt;", $A36))</f>
         <v>0</v>
       </c>
       <c r="J40" s="42"/>
@@ -20229,7 +20259,7 @@
         <v>17</v>
       </c>
       <c r="L40" s="53">
-        <f ca="1">SUMIFS('Trading History'!$AA$4:$AA961, 'Trading History'!$Y$4:$Y961, _xludf.CONCAT("&gt;", $A36))</f>
+        <f ca="1">SUMIFS('Trading History'!$AA$4:$AA962, 'Trading History'!$Y$4:$Y962, _xludf.CONCAT("&gt;", $A36))</f>
         <v>0</v>
       </c>
       <c r="M40" s="1"/>
@@ -20308,7 +20338,7 @@
         <v>18</v>
       </c>
       <c r="C43" s="45">
-        <f ca="1">SUMIFS('Trading History'!$N$4:$N961, 'Trading History'!$K$4:$K961, _xludf.CONCAT("&gt;", $A43))</f>
+        <f ca="1">SUMIFS('Trading History'!$N$4:$N962, 'Trading History'!$K$4:$K962, _xludf.CONCAT("&gt;", $A43))</f>
         <v>0</v>
       </c>
       <c r="D43" s="42"/>
@@ -20316,7 +20346,7 @@
         <v>66</v>
       </c>
       <c r="F43" s="45">
-        <f ca="1">IFERROR(SUMIFS('Trading History'!$R$4:$R961, 'Trading History'!$O$4:$O961, _xludf.CONCAT("&gt;", $A43)), 0)</f>
+        <f ca="1">IFERROR(SUMIFS('Trading History'!$R$4:$R962, 'Trading History'!$O$4:$O962, _xludf.CONCAT("&gt;", $A43)), 0)</f>
         <v>0</v>
       </c>
       <c r="G43" s="42"/>
@@ -20324,7 +20354,7 @@
         <v>67</v>
       </c>
       <c r="I43" s="45">
-        <f ca="1">SUMIFS('Trading History'!$V$4:$V961, 'Trading History'!$S$4:$S961, _xludf.CONCAT("&gt;", $A43))</f>
+        <f ca="1">SUMIFS('Trading History'!$V$4:$V962, 'Trading History'!$S$4:$S962, _xludf.CONCAT("&gt;", $A43))</f>
         <v>0</v>
       </c>
       <c r="J43" s="42"/>
@@ -20332,7 +20362,7 @@
         <v>18</v>
       </c>
       <c r="L43" s="45">
-        <f ca="1">SUMIFS('Trading History'!$AB$4:$AB961, 'Trading History'!$Y$4:$Y961, _xludf.CONCAT("&gt;", $A43))</f>
+        <f ca="1">SUMIFS('Trading History'!$AB$4:$AB962, 'Trading History'!$Y$4:$Y962, _xludf.CONCAT("&gt;", $A43))</f>
         <v>0</v>
       </c>
       <c r="M43" s="1"/>
@@ -20402,7 +20432,7 @@
         <v>16</v>
       </c>
       <c r="C45" s="53">
-        <f ca="1">SUMIFS('Trading History'!$L$4:$L961, 'Trading History'!$K$4:$K961, _xludf.CONCAT("&gt;", $A43))</f>
+        <f ca="1">SUMIFS('Trading History'!$L$4:$L962, 'Trading History'!$K$4:$K962, _xludf.CONCAT("&gt;", $A43))</f>
         <v>0</v>
       </c>
       <c r="D45" s="42"/>
@@ -20410,7 +20440,7 @@
         <v>71</v>
       </c>
       <c r="F45" s="53">
-        <f ca="1">SUMIFS('Trading History'!$P$4:$P961, 'Trading History'!$O$4:$O961, _xludf.CONCAT("&gt;", $A43))</f>
+        <f ca="1">SUMIFS('Trading History'!$P$4:$P962, 'Trading History'!$O$4:$O962, _xludf.CONCAT("&gt;", $A43))</f>
         <v>0</v>
       </c>
       <c r="G45" s="42"/>
@@ -20418,7 +20448,7 @@
         <v>72</v>
       </c>
       <c r="I45" s="53">
-        <f ca="1">SUMIFS('Trading History'!$T$4:$T961, 'Trading History'!$S$4:$S961, _xludf.CONCAT("&gt;", $A43))</f>
+        <f ca="1">SUMIFS('Trading History'!$T$4:$T962, 'Trading History'!$S$4:$S962, _xludf.CONCAT("&gt;", $A43))</f>
         <v>0</v>
       </c>
       <c r="J45" s="42"/>
@@ -20426,7 +20456,7 @@
         <v>16</v>
       </c>
       <c r="L45" s="53">
-        <f ca="1">SUMIFS('Trading History'!$Z$4:$Z961, 'Trading History'!$Y$4:$Y961, _xludf.CONCAT("&gt;", $A43))</f>
+        <f ca="1">SUMIFS('Trading History'!$Z$4:$Z962, 'Trading History'!$Y$4:$Y962, _xludf.CONCAT("&gt;", $A43))</f>
         <v>0</v>
       </c>
       <c r="M45" s="1"/>
@@ -20496,7 +20526,7 @@
         <v>17</v>
       </c>
       <c r="C47" s="53">
-        <f ca="1">SUMIFS('Trading History'!$M$4:$M961, 'Trading History'!$K$4:$K961, _xludf.CONCAT("&gt;", $A43))</f>
+        <f ca="1">SUMIFS('Trading History'!$M$4:$M962, 'Trading History'!$K$4:$K962, _xludf.CONCAT("&gt;", $A43))</f>
         <v>0</v>
       </c>
       <c r="D47" s="42"/>
@@ -20504,7 +20534,7 @@
         <v>76</v>
       </c>
       <c r="F47" s="53">
-        <f ca="1">SUMIFS('Trading History'!$Q$4:$Q961, 'Trading History'!$O$4:$O961, _xludf.CONCAT("&gt;", $A43))</f>
+        <f ca="1">SUMIFS('Trading History'!$Q$4:$Q962, 'Trading History'!$O$4:$O962, _xludf.CONCAT("&gt;", $A43))</f>
         <v>0</v>
       </c>
       <c r="G47" s="42"/>
@@ -20512,7 +20542,7 @@
         <v>77</v>
       </c>
       <c r="I47" s="53">
-        <f ca="1">SUMIFS('Trading History'!$U$4:$U961, 'Trading History'!$S$4:$S961, _xludf.CONCAT("&gt;", $A43))</f>
+        <f ca="1">SUMIFS('Trading History'!$U$4:$U962, 'Trading History'!$S$4:$S962, _xludf.CONCAT("&gt;", $A43))</f>
         <v>0</v>
       </c>
       <c r="J47" s="42"/>
@@ -20520,7 +20550,7 @@
         <v>17</v>
       </c>
       <c r="L47" s="53">
-        <f ca="1">SUMIFS('Trading History'!$AA$4:$AA961, 'Trading History'!$Y$4:$Y961, _xludf.CONCAT("&gt;", $A43))</f>
+        <f ca="1">SUMIFS('Trading History'!$AA$4:$AA962, 'Trading History'!$Y$4:$Y962, _xludf.CONCAT("&gt;", $A43))</f>
         <v>0</v>
       </c>
       <c r="M47" s="1"/>
@@ -20599,7 +20629,7 @@
         <v>18</v>
       </c>
       <c r="C50" s="45">
-        <f ca="1">SUMIFS('Trading History'!$N$4:$N961, 'Trading History'!$K$4:$K961, _xludf.CONCAT("&gt;", $A50))</f>
+        <f ca="1">SUMIFS('Trading History'!$N$4:$N962, 'Trading History'!$K$4:$K962, _xludf.CONCAT("&gt;", $A50))</f>
         <v>0</v>
       </c>
       <c r="D50" s="42"/>
@@ -20607,7 +20637,7 @@
         <v>66</v>
       </c>
       <c r="F50" s="45">
-        <f ca="1">IFERROR(SUMIFS('Trading History'!$R$4:$R961, 'Trading History'!$O$4:$O961, _xludf.CONCAT("&gt;", $A50)), 0)</f>
+        <f ca="1">IFERROR(SUMIFS('Trading History'!$R$4:$R962, 'Trading History'!$O$4:$O962, _xludf.CONCAT("&gt;", $A50)), 0)</f>
         <v>0</v>
       </c>
       <c r="G50" s="42"/>
@@ -20615,7 +20645,7 @@
         <v>67</v>
       </c>
       <c r="I50" s="45">
-        <f ca="1">SUMIFS('Trading History'!$V$4:$V961, 'Trading History'!$S$4:$S961, _xludf.CONCAT("&gt;", $A50))</f>
+        <f ca="1">SUMIFS('Trading History'!$V$4:$V962, 'Trading History'!$S$4:$S962, _xludf.CONCAT("&gt;", $A50))</f>
         <v>0</v>
       </c>
       <c r="J50" s="42"/>
@@ -20623,7 +20653,7 @@
         <v>18</v>
       </c>
       <c r="L50" s="45">
-        <f ca="1">SUMIFS('Trading History'!$AB$4:$AB961, 'Trading History'!$Y$4:$Y961, _xludf.CONCAT("&gt;", $A50))</f>
+        <f ca="1">SUMIFS('Trading History'!$AB$4:$AB962, 'Trading History'!$Y$4:$Y962, _xludf.CONCAT("&gt;", $A50))</f>
         <v>0</v>
       </c>
       <c r="M50" s="1"/>
@@ -20693,7 +20723,7 @@
         <v>16</v>
       </c>
       <c r="C52" s="53">
-        <f ca="1">SUMIFS('Trading History'!$L$4:$L961, 'Trading History'!$K$4:$K961, _xludf.CONCAT("&gt;", $A50))</f>
+        <f ca="1">SUMIFS('Trading History'!$L$4:$L962, 'Trading History'!$K$4:$K962, _xludf.CONCAT("&gt;", $A50))</f>
         <v>0</v>
       </c>
       <c r="D52" s="42"/>
@@ -20701,7 +20731,7 @@
         <v>71</v>
       </c>
       <c r="F52" s="53">
-        <f ca="1">SUMIFS('Trading History'!$P$4:$P961, 'Trading History'!$O$4:$O961, _xludf.CONCAT("&gt;", $A50))</f>
+        <f ca="1">SUMIFS('Trading History'!$P$4:$P962, 'Trading History'!$O$4:$O962, _xludf.CONCAT("&gt;", $A50))</f>
         <v>0</v>
       </c>
       <c r="G52" s="42"/>
@@ -20709,7 +20739,7 @@
         <v>72</v>
       </c>
       <c r="I52" s="53">
-        <f ca="1">SUMIFS('Trading History'!$T$4:$T961, 'Trading History'!$S$4:$S961, _xludf.CONCAT("&gt;", $A50))</f>
+        <f ca="1">SUMIFS('Trading History'!$T$4:$T962, 'Trading History'!$S$4:$S962, _xludf.CONCAT("&gt;", $A50))</f>
         <v>0</v>
       </c>
       <c r="J52" s="42"/>
@@ -20717,7 +20747,7 @@
         <v>16</v>
       </c>
       <c r="L52" s="53">
-        <f ca="1">SUMIFS('Trading History'!$Z$4:$Z961, 'Trading History'!$Y$4:$Y961, _xludf.CONCAT("&gt;", $A50))</f>
+        <f ca="1">SUMIFS('Trading History'!$Z$4:$Z962, 'Trading History'!$Y$4:$Y962, _xludf.CONCAT("&gt;", $A50))</f>
         <v>0</v>
       </c>
       <c r="M52" s="1"/>
@@ -20787,7 +20817,7 @@
         <v>17</v>
       </c>
       <c r="C54" s="53">
-        <f ca="1">SUMIFS('Trading History'!$M$4:$M961, 'Trading History'!$K$4:$K961, _xludf.CONCAT("&gt;", $A50))</f>
+        <f ca="1">SUMIFS('Trading History'!$M$4:$M962, 'Trading History'!$K$4:$K962, _xludf.CONCAT("&gt;", $A50))</f>
         <v>0</v>
       </c>
       <c r="D54" s="42"/>
@@ -20795,7 +20825,7 @@
         <v>76</v>
       </c>
       <c r="F54" s="53">
-        <f ca="1">SUMIFS('Trading History'!$Q$4:$Q961, 'Trading History'!$O$4:$O961, _xludf.CONCAT("&gt;", $A50))</f>
+        <f ca="1">SUMIFS('Trading History'!$Q$4:$Q962, 'Trading History'!$O$4:$O962, _xludf.CONCAT("&gt;", $A50))</f>
         <v>0</v>
       </c>
       <c r="G54" s="42"/>
@@ -20803,7 +20833,7 @@
         <v>77</v>
       </c>
       <c r="I54" s="53">
-        <f ca="1">SUMIFS('Trading History'!$U$4:$U961, 'Trading History'!$S$4:$S961, _xludf.CONCAT("&gt;", $A50))</f>
+        <f ca="1">SUMIFS('Trading History'!$U$4:$U962, 'Trading History'!$S$4:$S962, _xludf.CONCAT("&gt;", $A50))</f>
         <v>0</v>
       </c>
       <c r="J54" s="42"/>
@@ -20811,7 +20841,7 @@
         <v>17</v>
       </c>
       <c r="L54" s="53">
-        <f ca="1">SUMIFS('Trading History'!$AA$4:$AA961, 'Trading History'!$Y$4:$Y961, _xludf.CONCAT("&gt;", $A50))</f>
+        <f ca="1">SUMIFS('Trading History'!$AA$4:$AA962, 'Trading History'!$Y$4:$Y962, _xludf.CONCAT("&gt;", $A50))</f>
         <v>0</v>
       </c>
       <c r="M54" s="1"/>
@@ -20890,7 +20920,7 @@
         <v>18</v>
       </c>
       <c r="C57" s="45">
-        <f ca="1">SUMIFS('Trading History'!$N$4:$N961, 'Trading History'!$K$4:$K961, _xludf.CONCAT("&gt;", $A57))</f>
+        <f ca="1">SUMIFS('Trading History'!$N$4:$N962, 'Trading History'!$K$4:$K962, _xludf.CONCAT("&gt;", $A57))</f>
         <v>0</v>
       </c>
       <c r="D57" s="42"/>
@@ -20898,7 +20928,7 @@
         <v>66</v>
       </c>
       <c r="F57" s="45">
-        <f ca="1">IFERROR(SUMIFS('Trading History'!$R$4:$R961, 'Trading History'!$O$4:$O961, _xludf.CONCAT("&gt;", $A57)), 0)</f>
+        <f ca="1">IFERROR(SUMIFS('Trading History'!$R$4:$R962, 'Trading History'!$O$4:$O962, _xludf.CONCAT("&gt;", $A57)), 0)</f>
         <v>0</v>
       </c>
       <c r="G57" s="42"/>
@@ -20906,7 +20936,7 @@
         <v>67</v>
       </c>
       <c r="I57" s="45">
-        <f ca="1">SUMIFS('Trading History'!$V$4:$V961, 'Trading History'!$S$4:$S961, _xludf.CONCAT("&gt;", $A57))</f>
+        <f ca="1">SUMIFS('Trading History'!$V$4:$V962, 'Trading History'!$S$4:$S962, _xludf.CONCAT("&gt;", $A57))</f>
         <v>0</v>
       </c>
       <c r="J57" s="42"/>
@@ -20914,7 +20944,7 @@
         <v>18</v>
       </c>
       <c r="L57" s="45">
-        <f ca="1">SUMIFS('Trading History'!$AB$4:$AB961, 'Trading History'!$Y$4:$Y961, _xludf.CONCAT("&gt;", $A57))</f>
+        <f ca="1">SUMIFS('Trading History'!$AB$4:$AB962, 'Trading History'!$Y$4:$Y962, _xludf.CONCAT("&gt;", $A57))</f>
         <v>0</v>
       </c>
       <c r="M57" s="1"/>
@@ -20984,7 +21014,7 @@
         <v>16</v>
       </c>
       <c r="C59" s="53">
-        <f ca="1">SUMIFS('Trading History'!$L$4:$L961, 'Trading History'!$K$4:$K961, _xludf.CONCAT("&gt;", $A57))</f>
+        <f ca="1">SUMIFS('Trading History'!$L$4:$L962, 'Trading History'!$K$4:$K962, _xludf.CONCAT("&gt;", $A57))</f>
         <v>0</v>
       </c>
       <c r="D59" s="42"/>
@@ -20992,7 +21022,7 @@
         <v>71</v>
       </c>
       <c r="F59" s="53">
-        <f ca="1">SUMIFS('Trading History'!$P$4:$P961, 'Trading History'!$O$4:$O961, _xludf.CONCAT("&gt;", $A57))</f>
+        <f ca="1">SUMIFS('Trading History'!$P$4:$P962, 'Trading History'!$O$4:$O962, _xludf.CONCAT("&gt;", $A57))</f>
         <v>0</v>
       </c>
       <c r="G59" s="42"/>
@@ -21000,7 +21030,7 @@
         <v>72</v>
       </c>
       <c r="I59" s="53">
-        <f ca="1">SUMIFS('Trading History'!$T$4:$T961, 'Trading History'!$S$4:$S961, _xludf.CONCAT("&gt;", $A57))</f>
+        <f ca="1">SUMIFS('Trading History'!$T$4:$T962, 'Trading History'!$S$4:$S962, _xludf.CONCAT("&gt;", $A57))</f>
         <v>0</v>
       </c>
       <c r="J59" s="42"/>
@@ -21008,7 +21038,7 @@
         <v>16</v>
       </c>
       <c r="L59" s="53">
-        <f ca="1">SUMIFS('Trading History'!$Z$4:$Z961, 'Trading History'!$Y$4:$Y961, _xludf.CONCAT("&gt;", $A57))</f>
+        <f ca="1">SUMIFS('Trading History'!$Z$4:$Z962, 'Trading History'!$Y$4:$Y962, _xludf.CONCAT("&gt;", $A57))</f>
         <v>0</v>
       </c>
       <c r="M59" s="1"/>
@@ -21078,7 +21108,7 @@
         <v>17</v>
       </c>
       <c r="C61" s="53">
-        <f ca="1">SUMIFS('Trading History'!$M$4:$M961, 'Trading History'!$K$4:$K961, _xludf.CONCAT("&gt;", $A57))</f>
+        <f ca="1">SUMIFS('Trading History'!$M$4:$M962, 'Trading History'!$K$4:$K962, _xludf.CONCAT("&gt;", $A57))</f>
         <v>0</v>
       </c>
       <c r="D61" s="42"/>
@@ -21086,7 +21116,7 @@
         <v>76</v>
       </c>
       <c r="F61" s="53">
-        <f ca="1">SUMIFS('Trading History'!$Q$4:$Q961, 'Trading History'!$O$4:$O961, _xludf.CONCAT("&gt;", $A57))</f>
+        <f ca="1">SUMIFS('Trading History'!$Q$4:$Q962, 'Trading History'!$O$4:$O962, _xludf.CONCAT("&gt;", $A57))</f>
         <v>0</v>
       </c>
       <c r="G61" s="42"/>
@@ -21094,7 +21124,7 @@
         <v>77</v>
       </c>
       <c r="I61" s="53">
-        <f ca="1">SUMIFS('Trading History'!$U$4:$U961, 'Trading History'!$S$4:$S961, _xludf.CONCAT("&gt;", $A57))</f>
+        <f ca="1">SUMIFS('Trading History'!$U$4:$U962, 'Trading History'!$S$4:$S962, _xludf.CONCAT("&gt;", $A57))</f>
         <v>0</v>
       </c>
       <c r="J61" s="42"/>
@@ -21102,7 +21132,7 @@
         <v>17</v>
       </c>
       <c r="L61" s="53">
-        <f ca="1">SUMIFS('Trading History'!$AA$4:$AA961, 'Trading History'!$Y$4:$Y961, _xludf.CONCAT("&gt;", $A57))</f>
+        <f ca="1">SUMIFS('Trading History'!$AA$4:$AA962, 'Trading History'!$Y$4:$Y962, _xludf.CONCAT("&gt;", $A57))</f>
         <v>0</v>
       </c>
       <c r="M61" s="1"/>
@@ -21181,7 +21211,7 @@
         <v>18</v>
       </c>
       <c r="C64" s="45">
-        <f ca="1">SUMIFS('Trading History'!$N$4:$N961, 'Trading History'!$K$4:$K961, _xludf.CONCAT("&gt;", $A64))</f>
+        <f ca="1">SUMIFS('Trading History'!$N$4:$N962, 'Trading History'!$K$4:$K962, _xludf.CONCAT("&gt;", $A64))</f>
         <v>0</v>
       </c>
       <c r="D64" s="42"/>
@@ -21189,7 +21219,7 @@
         <v>66</v>
       </c>
       <c r="F64" s="45">
-        <f ca="1">IFERROR(SUMIFS('Trading History'!$R$4:$R961, 'Trading History'!$O$4:$O961, _xludf.CONCAT("&gt;", $A64)), 0)</f>
+        <f ca="1">IFERROR(SUMIFS('Trading History'!$R$4:$R962, 'Trading History'!$O$4:$O962, _xludf.CONCAT("&gt;", $A64)), 0)</f>
         <v>0</v>
       </c>
       <c r="G64" s="42"/>
@@ -21197,7 +21227,7 @@
         <v>67</v>
       </c>
       <c r="I64" s="45">
-        <f ca="1">SUMIFS('Trading History'!$V$4:$V961, 'Trading History'!$S$4:$S961, _xludf.CONCAT("&gt;", $A64))</f>
+        <f ca="1">SUMIFS('Trading History'!$V$4:$V962, 'Trading History'!$S$4:$S962, _xludf.CONCAT("&gt;", $A64))</f>
         <v>0</v>
       </c>
       <c r="J64" s="42"/>
@@ -21205,7 +21235,7 @@
         <v>18</v>
       </c>
       <c r="L64" s="45">
-        <f ca="1">SUMIFS('Trading History'!$AB$4:$AB961, 'Trading History'!$Y$4:$Y961, _xludf.CONCAT("&gt;", $A64))</f>
+        <f ca="1">SUMIFS('Trading History'!$AB$4:$AB962, 'Trading History'!$Y$4:$Y962, _xludf.CONCAT("&gt;", $A64))</f>
         <v>0</v>
       </c>
       <c r="M64" s="1"/>
@@ -21275,7 +21305,7 @@
         <v>16</v>
       </c>
       <c r="C66" s="53">
-        <f ca="1">SUMIFS('Trading History'!$L$4:$L961, 'Trading History'!$K$4:$K961, _xludf.CONCAT("&gt;", $A64))</f>
+        <f ca="1">SUMIFS('Trading History'!$L$4:$L962, 'Trading History'!$K$4:$K962, _xludf.CONCAT("&gt;", $A64))</f>
         <v>0</v>
       </c>
       <c r="D66" s="42"/>
@@ -21283,7 +21313,7 @@
         <v>71</v>
       </c>
       <c r="F66" s="53">
-        <f ca="1">SUMIFS('Trading History'!$P$4:$P961, 'Trading History'!$O$4:$O961, _xludf.CONCAT("&gt;", $A64))</f>
+        <f ca="1">SUMIFS('Trading History'!$P$4:$P962, 'Trading History'!$O$4:$O962, _xludf.CONCAT("&gt;", $A64))</f>
         <v>0</v>
       </c>
       <c r="G66" s="42"/>
@@ -21291,7 +21321,7 @@
         <v>72</v>
       </c>
       <c r="I66" s="53">
-        <f ca="1">SUMIFS('Trading History'!$T$4:$T961, 'Trading History'!$S$4:$S961, _xludf.CONCAT("&gt;", $A64))</f>
+        <f ca="1">SUMIFS('Trading History'!$T$4:$T962, 'Trading History'!$S$4:$S962, _xludf.CONCAT("&gt;", $A64))</f>
         <v>0</v>
       </c>
       <c r="J66" s="42"/>
@@ -21299,7 +21329,7 @@
         <v>16</v>
       </c>
       <c r="L66" s="53">
-        <f ca="1">SUMIFS('Trading History'!$Z$4:$Z961, 'Trading History'!$Y$4:$Y961, _xludf.CONCAT("&gt;", $A64))</f>
+        <f ca="1">SUMIFS('Trading History'!$Z$4:$Z962, 'Trading History'!$Y$4:$Y962, _xludf.CONCAT("&gt;", $A64))</f>
         <v>0</v>
       </c>
       <c r="M66" s="1"/>
@@ -21369,7 +21399,7 @@
         <v>17</v>
       </c>
       <c r="C68" s="53">
-        <f ca="1">SUMIFS('Trading History'!$M$4:$M961, 'Trading History'!$K$4:$K961, _xludf.CONCAT("&gt;", $A64))</f>
+        <f ca="1">SUMIFS('Trading History'!$M$4:$M962, 'Trading History'!$K$4:$K962, _xludf.CONCAT("&gt;", $A64))</f>
         <v>0</v>
       </c>
       <c r="D68" s="42"/>
@@ -21377,7 +21407,7 @@
         <v>76</v>
       </c>
       <c r="F68" s="53">
-        <f ca="1">SUMIFS('Trading History'!$Q$4:$Q961, 'Trading History'!$O$4:$O961, _xludf.CONCAT("&gt;", $A64))</f>
+        <f ca="1">SUMIFS('Trading History'!$Q$4:$Q962, 'Trading History'!$O$4:$O962, _xludf.CONCAT("&gt;", $A64))</f>
         <v>0</v>
       </c>
       <c r="G68" s="42"/>
@@ -21385,7 +21415,7 @@
         <v>77</v>
       </c>
       <c r="I68" s="53">
-        <f ca="1">SUMIFS('Trading History'!$U$4:$U961, 'Trading History'!$S$4:$S961, _xludf.CONCAT("&gt;", $A64))</f>
+        <f ca="1">SUMIFS('Trading History'!$U$4:$U962, 'Trading History'!$S$4:$S962, _xludf.CONCAT("&gt;", $A64))</f>
         <v>0</v>
       </c>
       <c r="J68" s="42"/>
@@ -21393,7 +21423,7 @@
         <v>17</v>
       </c>
       <c r="L68" s="53">
-        <f ca="1">SUMIFS('Trading History'!$AA$4:$AA961, 'Trading History'!$Y$4:$Y961, _xludf.CONCAT("&gt;", $A64))</f>
+        <f ca="1">SUMIFS('Trading History'!$AA$4:$AA962, 'Trading History'!$Y$4:$Y962, _xludf.CONCAT("&gt;", $A64))</f>
         <v>0</v>
       </c>
       <c r="M68" s="1"/>
@@ -21472,7 +21502,7 @@
         <v>18</v>
       </c>
       <c r="C71" s="45">
-        <f ca="1">SUMIFS('Trading History'!$N$4:$N961, 'Trading History'!$K$4:$K961, _xludf.CONCAT("&gt;", $A71))</f>
+        <f ca="1">SUMIFS('Trading History'!$N$4:$N962, 'Trading History'!$K$4:$K962, _xludf.CONCAT("&gt;", $A71))</f>
         <v>0</v>
       </c>
       <c r="D71" s="42"/>
@@ -21480,7 +21510,7 @@
         <v>66</v>
       </c>
       <c r="F71" s="45">
-        <f ca="1">IFERROR(SUMIFS('Trading History'!$R$4:$R961, 'Trading History'!$O$4:$O961, _xludf.CONCAT("&gt;", $A71)), 0)</f>
+        <f ca="1">IFERROR(SUMIFS('Trading History'!$R$4:$R962, 'Trading History'!$O$4:$O962, _xludf.CONCAT("&gt;", $A71)), 0)</f>
         <v>0</v>
       </c>
       <c r="G71" s="42"/>
@@ -21488,7 +21518,7 @@
         <v>67</v>
       </c>
       <c r="I71" s="45">
-        <f ca="1">SUMIFS('Trading History'!$V$4:$V961, 'Trading History'!$S$4:$S961, _xludf.CONCAT("&gt;", $A71))</f>
+        <f ca="1">SUMIFS('Trading History'!$V$4:$V962, 'Trading History'!$S$4:$S962, _xludf.CONCAT("&gt;", $A71))</f>
         <v>0</v>
       </c>
       <c r="J71" s="42"/>
@@ -21496,7 +21526,7 @@
         <v>18</v>
       </c>
       <c r="L71" s="45">
-        <f ca="1">SUMIFS('Trading History'!$AB$4:$AB961, 'Trading History'!$Y$4:$Y961, _xludf.CONCAT("&gt;", $A71))</f>
+        <f ca="1">SUMIFS('Trading History'!$AB$4:$AB962, 'Trading History'!$Y$4:$Y962, _xludf.CONCAT("&gt;", $A71))</f>
         <v>0</v>
       </c>
       <c r="M71" s="1"/>
@@ -21566,7 +21596,7 @@
         <v>16</v>
       </c>
       <c r="C73" s="53">
-        <f ca="1">SUMIFS('Trading History'!$L$4:$L961, 'Trading History'!$K$4:$K961, _xludf.CONCAT("&gt;", $A71))</f>
+        <f ca="1">SUMIFS('Trading History'!$L$4:$L962, 'Trading History'!$K$4:$K962, _xludf.CONCAT("&gt;", $A71))</f>
         <v>0</v>
       </c>
       <c r="D73" s="42"/>
@@ -21574,7 +21604,7 @@
         <v>71</v>
       </c>
       <c r="F73" s="53">
-        <f ca="1">SUMIFS('Trading History'!$P$4:$P961, 'Trading History'!$O$4:$O961, _xludf.CONCAT("&gt;", $A71))</f>
+        <f ca="1">SUMIFS('Trading History'!$P$4:$P962, 'Trading History'!$O$4:$O962, _xludf.CONCAT("&gt;", $A71))</f>
         <v>0</v>
       </c>
       <c r="G73" s="42"/>
@@ -21582,7 +21612,7 @@
         <v>72</v>
       </c>
       <c r="I73" s="53">
-        <f ca="1">SUMIFS('Trading History'!$T$4:$T961, 'Trading History'!$S$4:$S961, _xludf.CONCAT("&gt;", $A71))</f>
+        <f ca="1">SUMIFS('Trading History'!$T$4:$T962, 'Trading History'!$S$4:$S962, _xludf.CONCAT("&gt;", $A71))</f>
         <v>0</v>
       </c>
       <c r="J73" s="42"/>
@@ -21590,7 +21620,7 @@
         <v>16</v>
       </c>
       <c r="L73" s="53">
-        <f ca="1">SUMIFS('Trading History'!$Z$4:$Z961, 'Trading History'!$Y$4:$Y961, _xludf.CONCAT("&gt;", $A71))</f>
+        <f ca="1">SUMIFS('Trading History'!$Z$4:$Z962, 'Trading History'!$Y$4:$Y962, _xludf.CONCAT("&gt;", $A71))</f>
         <v>0</v>
       </c>
       <c r="M73" s="1"/>
@@ -21660,7 +21690,7 @@
         <v>17</v>
       </c>
       <c r="C75" s="53">
-        <f ca="1">SUMIFS('Trading History'!$M$4:$M961, 'Trading History'!$K$4:$K961, _xludf.CONCAT("&gt;", $A71))</f>
+        <f ca="1">SUMIFS('Trading History'!$M$4:$M962, 'Trading History'!$K$4:$K962, _xludf.CONCAT("&gt;", $A71))</f>
         <v>0</v>
       </c>
       <c r="D75" s="42"/>
@@ -21668,7 +21698,7 @@
         <v>76</v>
       </c>
       <c r="F75" s="53">
-        <f ca="1">SUMIFS('Trading History'!$Q$4:$Q961, 'Trading History'!$O$4:$O961, _xludf.CONCAT("&gt;", $A71))</f>
+        <f ca="1">SUMIFS('Trading History'!$Q$4:$Q962, 'Trading History'!$O$4:$O962, _xludf.CONCAT("&gt;", $A71))</f>
         <v>0</v>
       </c>
       <c r="G75" s="42"/>
@@ -21676,7 +21706,7 @@
         <v>77</v>
       </c>
       <c r="I75" s="53">
-        <f ca="1">SUMIFS('Trading History'!$U$4:$U961, 'Trading History'!$S$4:$S961, _xludf.CONCAT("&gt;", $A71))</f>
+        <f ca="1">SUMIFS('Trading History'!$U$4:$U962, 'Trading History'!$S$4:$S962, _xludf.CONCAT("&gt;", $A71))</f>
         <v>0</v>
       </c>
       <c r="J75" s="42"/>
@@ -21684,7 +21714,7 @@
         <v>17</v>
       </c>
       <c r="L75" s="53">
-        <f ca="1">SUMIFS('Trading History'!$AA$4:$AA961, 'Trading History'!$Y$4:$Y961, _xludf.CONCAT("&gt;", $A71))</f>
+        <f ca="1">SUMIFS('Trading History'!$AA$4:$AA962, 'Trading History'!$Y$4:$Y962, _xludf.CONCAT("&gt;", $A71))</f>
         <v>0</v>
       </c>
       <c r="M75" s="1"/>
@@ -21763,7 +21793,7 @@
         <v>18</v>
       </c>
       <c r="C78" s="45">
-        <f ca="1">SUMIFS('Trading History'!$N$4:$N961, 'Trading History'!$K$4:$K961, _xludf.CONCAT("&gt;", $A78))</f>
+        <f ca="1">SUMIFS('Trading History'!$N$4:$N962, 'Trading History'!$K$4:$K962, _xludf.CONCAT("&gt;", $A78))</f>
         <v>0</v>
       </c>
       <c r="D78" s="42"/>
@@ -21771,7 +21801,7 @@
         <v>66</v>
       </c>
       <c r="F78" s="45">
-        <f ca="1">IFERROR(SUMIFS('Trading History'!$R$4:$R961, 'Trading History'!$O$4:$O961, _xludf.CONCAT("&gt;", $A78)), 0)</f>
+        <f ca="1">IFERROR(SUMIFS('Trading History'!$R$4:$R962, 'Trading History'!$O$4:$O962, _xludf.CONCAT("&gt;", $A78)), 0)</f>
         <v>0</v>
       </c>
       <c r="G78" s="42"/>
@@ -21779,7 +21809,7 @@
         <v>67</v>
       </c>
       <c r="I78" s="45">
-        <f ca="1">SUMIFS('Trading History'!$V$4:$V961, 'Trading History'!$S$4:$S961, _xludf.CONCAT("&gt;", $A78))</f>
+        <f ca="1">SUMIFS('Trading History'!$V$4:$V962, 'Trading History'!$S$4:$S962, _xludf.CONCAT("&gt;", $A78))</f>
         <v>0</v>
       </c>
       <c r="J78" s="42"/>
@@ -21787,7 +21817,7 @@
         <v>18</v>
       </c>
       <c r="L78" s="45">
-        <f ca="1">SUMIFS('Trading History'!$AB$4:$AB961, 'Trading History'!$Y$4:$Y961, _xludf.CONCAT("&gt;", $A78))</f>
+        <f ca="1">SUMIFS('Trading History'!$AB$4:$AB962, 'Trading History'!$Y$4:$Y962, _xludf.CONCAT("&gt;", $A78))</f>
         <v>0</v>
       </c>
       <c r="M78" s="1"/>
@@ -21857,7 +21887,7 @@
         <v>16</v>
       </c>
       <c r="C80" s="53">
-        <f ca="1">SUMIFS('Trading History'!$L$4:$L961, 'Trading History'!$K$4:$K961, _xludf.CONCAT("&gt;", $A78))</f>
+        <f ca="1">SUMIFS('Trading History'!$L$4:$L962, 'Trading History'!$K$4:$K962, _xludf.CONCAT("&gt;", $A78))</f>
         <v>0</v>
       </c>
       <c r="D80" s="42"/>
@@ -21865,7 +21895,7 @@
         <v>71</v>
       </c>
       <c r="F80" s="53">
-        <f ca="1">SUMIFS('Trading History'!$P$4:$P961, 'Trading History'!$O$4:$O961, _xludf.CONCAT("&gt;", $A78))</f>
+        <f ca="1">SUMIFS('Trading History'!$P$4:$P962, 'Trading History'!$O$4:$O962, _xludf.CONCAT("&gt;", $A78))</f>
         <v>0</v>
       </c>
       <c r="G80" s="42"/>
@@ -21873,7 +21903,7 @@
         <v>72</v>
       </c>
       <c r="I80" s="53">
-        <f ca="1">SUMIFS('Trading History'!$T$4:$T961, 'Trading History'!$S$4:$S961, _xludf.CONCAT("&gt;", $A78))</f>
+        <f ca="1">SUMIFS('Trading History'!$T$4:$T962, 'Trading History'!$S$4:$S962, _xludf.CONCAT("&gt;", $A78))</f>
         <v>0</v>
       </c>
       <c r="J80" s="42"/>
@@ -21881,7 +21911,7 @@
         <v>16</v>
       </c>
       <c r="L80" s="53">
-        <f ca="1">SUMIFS('Trading History'!$Z$4:$Z961, 'Trading History'!$Y$4:$Y961, _xludf.CONCAT("&gt;", $A78))</f>
+        <f ca="1">SUMIFS('Trading History'!$Z$4:$Z962, 'Trading History'!$Y$4:$Y962, _xludf.CONCAT("&gt;", $A78))</f>
         <v>0</v>
       </c>
       <c r="M80" s="1"/>
@@ -21951,7 +21981,7 @@
         <v>17</v>
       </c>
       <c r="C82" s="53">
-        <f ca="1">SUMIFS('Trading History'!$M$4:$M961, 'Trading History'!$K$4:$K961, _xludf.CONCAT("&gt;", $A78))</f>
+        <f ca="1">SUMIFS('Trading History'!$M$4:$M962, 'Trading History'!$K$4:$K962, _xludf.CONCAT("&gt;", $A78))</f>
         <v>0</v>
       </c>
       <c r="D82" s="42"/>
@@ -21959,7 +21989,7 @@
         <v>76</v>
       </c>
       <c r="F82" s="53">
-        <f ca="1">SUMIFS('Trading History'!$Q$4:$Q961, 'Trading History'!$O$4:$O961, _xludf.CONCAT("&gt;", $A78))</f>
+        <f ca="1">SUMIFS('Trading History'!$Q$4:$Q962, 'Trading History'!$O$4:$O962, _xludf.CONCAT("&gt;", $A78))</f>
         <v>0</v>
       </c>
       <c r="G82" s="42"/>
@@ -21967,7 +21997,7 @@
         <v>77</v>
       </c>
       <c r="I82" s="53">
-        <f ca="1">SUMIFS('Trading History'!$U$4:$U961, 'Trading History'!$S$4:$S961, _xludf.CONCAT("&gt;", $A78))</f>
+        <f ca="1">SUMIFS('Trading History'!$U$4:$U962, 'Trading History'!$S$4:$S962, _xludf.CONCAT("&gt;", $A78))</f>
         <v>0</v>
       </c>
       <c r="J82" s="42"/>
@@ -21975,7 +22005,7 @@
         <v>17</v>
       </c>
       <c r="L82" s="53">
-        <f ca="1">SUMIFS('Trading History'!$AA$4:$AA961, 'Trading History'!$Y$4:$Y961, _xludf.CONCAT("&gt;", $A78))</f>
+        <f ca="1">SUMIFS('Trading History'!$AA$4:$AA962, 'Trading History'!$Y$4:$Y962, _xludf.CONCAT("&gt;", $A78))</f>
         <v>0</v>
       </c>
       <c r="M82" s="1"/>
@@ -22054,7 +22084,7 @@
         <v>18</v>
       </c>
       <c r="C85" s="45">
-        <f ca="1">SUMIFS('Trading History'!$N$4:$N961, 'Trading History'!$K$4:$K961, _xludf.CONCAT("&gt;", $A85))</f>
+        <f ca="1">SUMIFS('Trading History'!$N$4:$N962, 'Trading History'!$K$4:$K962, _xludf.CONCAT("&gt;", $A85))</f>
         <v>0</v>
       </c>
       <c r="D85" s="42"/>
@@ -22062,7 +22092,7 @@
         <v>66</v>
       </c>
       <c r="F85" s="45">
-        <f ca="1">IFERROR(SUMIFS('Trading History'!$R$4:$R961, 'Trading History'!$O$4:$O961, _xludf.CONCAT("&gt;", $A85)), 0)</f>
+        <f ca="1">IFERROR(SUMIFS('Trading History'!$R$4:$R962, 'Trading History'!$O$4:$O962, _xludf.CONCAT("&gt;", $A85)), 0)</f>
         <v>0</v>
       </c>
       <c r="G85" s="42"/>
@@ -22070,7 +22100,7 @@
         <v>67</v>
       </c>
       <c r="I85" s="45">
-        <f ca="1">SUMIFS('Trading History'!$V$4:$V961, 'Trading History'!$S$4:$S961, _xludf.CONCAT("&gt;", $A85))</f>
+        <f ca="1">SUMIFS('Trading History'!$V$4:$V962, 'Trading History'!$S$4:$S962, _xludf.CONCAT("&gt;", $A85))</f>
         <v>0</v>
       </c>
       <c r="J85" s="42"/>
@@ -22078,7 +22108,7 @@
         <v>18</v>
       </c>
       <c r="L85" s="45">
-        <f ca="1">SUMIFS('Trading History'!$AB$4:$AB961, 'Trading History'!$Y$4:$Y961, _xludf.CONCAT("&gt;", $A85))</f>
+        <f ca="1">SUMIFS('Trading History'!$AB$4:$AB962, 'Trading History'!$Y$4:$Y962, _xludf.CONCAT("&gt;", $A85))</f>
         <v>0</v>
       </c>
       <c r="M85" s="1"/>
@@ -22148,7 +22178,7 @@
         <v>16</v>
       </c>
       <c r="C87" s="53">
-        <f ca="1">SUMIFS('Trading History'!$L$4:$L961, 'Trading History'!$K$4:$K961, _xludf.CONCAT("&gt;", $A85))</f>
+        <f ca="1">SUMIFS('Trading History'!$L$4:$L962, 'Trading History'!$K$4:$K962, _xludf.CONCAT("&gt;", $A85))</f>
         <v>0</v>
       </c>
       <c r="D87" s="42"/>
@@ -22156,7 +22186,7 @@
         <v>71</v>
       </c>
       <c r="F87" s="53">
-        <f ca="1">SUMIFS('Trading History'!$P$4:$P961, 'Trading History'!$O$4:$O961, _xludf.CONCAT("&gt;", $A85))</f>
+        <f ca="1">SUMIFS('Trading History'!$P$4:$P962, 'Trading History'!$O$4:$O962, _xludf.CONCAT("&gt;", $A85))</f>
         <v>0</v>
       </c>
       <c r="G87" s="42"/>
@@ -22164,7 +22194,7 @@
         <v>72</v>
       </c>
       <c r="I87" s="53">
-        <f ca="1">SUMIFS('Trading History'!$T$4:$T961, 'Trading History'!$S$4:$S961, _xludf.CONCAT("&gt;", $A85))</f>
+        <f ca="1">SUMIFS('Trading History'!$T$4:$T962, 'Trading History'!$S$4:$S962, _xludf.CONCAT("&gt;", $A85))</f>
         <v>0</v>
       </c>
       <c r="J87" s="42"/>
@@ -22172,7 +22202,7 @@
         <v>16</v>
       </c>
       <c r="L87" s="53">
-        <f ca="1">SUMIFS('Trading History'!$Z$4:$Z961, 'Trading History'!$Y$4:$Y961, _xludf.CONCAT("&gt;", $A85))</f>
+        <f ca="1">SUMIFS('Trading History'!$Z$4:$Z962, 'Trading History'!$Y$4:$Y962, _xludf.CONCAT("&gt;", $A85))</f>
         <v>0</v>
       </c>
       <c r="M87" s="1"/>
@@ -22242,7 +22272,7 @@
         <v>17</v>
       </c>
       <c r="C89" s="53">
-        <f ca="1">SUMIFS('Trading History'!$M$4:$M961, 'Trading History'!$K$4:$K961, _xludf.CONCAT("&gt;", $A85))</f>
+        <f ca="1">SUMIFS('Trading History'!$M$4:$M962, 'Trading History'!$K$4:$K962, _xludf.CONCAT("&gt;", $A85))</f>
         <v>0</v>
       </c>
       <c r="D89" s="42"/>
@@ -22250,7 +22280,7 @@
         <v>76</v>
       </c>
       <c r="F89" s="53">
-        <f ca="1">SUMIFS('Trading History'!$Q$4:$Q961, 'Trading History'!$O$4:$O961, _xludf.CONCAT("&gt;", $A85))</f>
+        <f ca="1">SUMIFS('Trading History'!$Q$4:$Q962, 'Trading History'!$O$4:$O962, _xludf.CONCAT("&gt;", $A85))</f>
         <v>0</v>
       </c>
       <c r="G89" s="42"/>
@@ -22258,7 +22288,7 @@
         <v>77</v>
       </c>
       <c r="I89" s="53">
-        <f ca="1">SUMIFS('Trading History'!$U$4:$U961, 'Trading History'!$S$4:$S961, _xludf.CONCAT("&gt;", $A85))</f>
+        <f ca="1">SUMIFS('Trading History'!$U$4:$U962, 'Trading History'!$S$4:$S962, _xludf.CONCAT("&gt;", $A85))</f>
         <v>0</v>
       </c>
       <c r="J89" s="42"/>
@@ -22266,7 +22296,7 @@
         <v>17</v>
       </c>
       <c r="L89" s="53">
-        <f ca="1">SUMIFS('Trading History'!$AA$4:$AA961, 'Trading History'!$Y$4:$Y961, _xludf.CONCAT("&gt;", $A85))</f>
+        <f ca="1">SUMIFS('Trading History'!$AA$4:$AA962, 'Trading History'!$Y$4:$Y962, _xludf.CONCAT("&gt;", $A85))</f>
         <v>0</v>
       </c>
       <c r="M89" s="1"/>

</xml_diff>